<commit_message>
Added sankey sensitivity analysis and updated sankey design
</commit_message>
<xml_diff>
--- a/data/glass_paper.xlsx
+++ b/data/glass_paper.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Desktop\python\glass-paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Desktop\python\glass-paper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FDF205-2F26-40CF-A064-420585C8F6F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D457E642-3813-4F98-9106-A06B99EB67CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{1AC0E601-1297-4C8D-8E5F-6A8C787FDED8}"/>
+    <workbookView xWindow="20370" yWindow="-5925" windowWidth="30960" windowHeight="16920" activeTab="3" xr2:uid="{1AC0E601-1297-4C8D-8E5F-6A8C787FDED8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="108">
   <si>
     <t>Global production of glass</t>
   </si>
@@ -182,9 +182,6 @@
     <t>Global Cont Recycling Rate</t>
   </si>
   <si>
-    <t>Global Cont Landfill Rate</t>
-  </si>
-  <si>
     <t>%Cullet in Batch</t>
   </si>
   <si>
@@ -291,16 +288,89 @@
   </si>
   <si>
     <t>Global flat glass production (final number) [Mt]</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>variation</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>gamma_1</t>
+  </si>
+  <si>
+    <t>gamma_2</t>
+  </si>
+  <si>
+    <t>delta_11</t>
+  </si>
+  <si>
+    <t>delta_12</t>
+  </si>
+  <si>
+    <t>delta_13</t>
+  </si>
+  <si>
+    <t>delta_21</t>
+  </si>
+  <si>
+    <t>delta_22</t>
+  </si>
+  <si>
+    <t>delta_23</t>
+  </si>
+  <si>
+    <t>epsilon</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Container glass melting</t>
+  </si>
+  <si>
+    <t>Flat glass melting</t>
+  </si>
+  <si>
+    <t>Container glass forming</t>
+  </si>
+  <si>
+    <t>Flat glass forming</t>
+  </si>
+  <si>
+    <t>Use of flat glass (automotive)</t>
+  </si>
+  <si>
+    <t>Use of flat glass (other)</t>
+  </si>
+  <si>
+    <t>Use of container glass (other)</t>
+  </si>
+  <si>
+    <t>Use of container glass (beverages)</t>
+  </si>
+  <si>
+    <t>Use of container glass (food)</t>
+  </si>
+  <si>
+    <t>Disposal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,6 +382,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -334,11 +411,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -346,10 +424,14 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -664,7 +746,7 @@
   <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +853,7 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3">
         <v>2014</v>
@@ -780,12 +862,12 @@
         <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4">
         <v>2007</v>
@@ -794,12 +876,12 @@
         <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5">
         <v>2007</v>
@@ -814,7 +896,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6">
         <v>2014</v>
@@ -829,7 +911,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7">
         <v>2014</v>
@@ -844,7 +926,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8">
         <v>2007</v>
@@ -858,7 +940,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9">
         <v>2014</v>
@@ -872,7 +954,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10">
         <v>2007</v>
@@ -886,7 +968,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11">
         <v>2014</v>
@@ -900,7 +982,7 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C13">
         <v>2014</v>
@@ -1173,7 +1255,7 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C19">
         <v>2014</v>
@@ -1201,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11B3549B-C2AB-4D75-AB88-A04A3C1A4639}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:AE41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z44" sqref="Z44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,18 +1296,18 @@
     <col min="7" max="7" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
         <v>68</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>70</v>
-      </c>
-      <c r="D1" t="s">
-        <v>71</v>
       </c>
       <c r="G1" t="s">
         <v>32</v>
@@ -1233,19 +1315,43 @@
       <c r="H1" s="5">
         <v>0.22409999999999999</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S1" t="s">
+        <v>84</v>
+      </c>
+      <c r="T1" t="s">
+        <v>86</v>
+      </c>
+      <c r="U1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
         <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
       </c>
       <c r="D2" s="4">
-        <f>(('Flat glass'!D19+D12))*H1</f>
+        <f>(('Flat glass'!$D$19+D11))*$H$1</f>
         <v>18.776050481185038</v>
       </c>
       <c r="G2" t="s">
@@ -1254,19 +1360,51 @@
       <c r="H2" s="5">
         <v>0.14069999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N2" s="4">
+        <f>(('Flat glass'!$D$19+N11))*$H$1</f>
+        <v>18.556524578213157</v>
+      </c>
+      <c r="O2" s="4">
+        <f>(('Flat glass'!$D$19+O11))*$H$1</f>
+        <v>18.776050481185038</v>
+      </c>
+      <c r="P2" s="4">
+        <f>(('Flat glass'!$D$19+P11))*$H$1</f>
+        <v>18.776050481185038</v>
+      </c>
+      <c r="Q2" s="4">
+        <f>(('Flat glass'!$D$19+Q11))*$H$1</f>
+        <v>18.776050481185038</v>
+      </c>
+      <c r="S2" s="8">
+        <f>N2/$D2</f>
+        <v>0.98830819595463582</v>
+      </c>
+      <c r="T2" s="8">
+        <f>O2/$D2</f>
+        <v>1</v>
+      </c>
+      <c r="U2" s="8">
+        <f>P2/$D2</f>
+        <v>1</v>
+      </c>
+      <c r="V2" s="8">
+        <f>Q2/$D2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
         <v>72</v>
-      </c>
-      <c r="B3" t="s">
-        <v>73</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="4">
-        <f>(('Flat glass'!D19+D12))*H3</f>
+        <f>(('Flat glass'!$D$19+D11))*$H$3</f>
         <v>53.219755759253616</v>
       </c>
       <c r="G3" t="s">
@@ -1275,20 +1413,55 @@
       <c r="H3" s="5">
         <v>0.63519999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N3" s="4">
+        <f>(('Flat glass'!$D$19+N11))*$H$3</f>
+        <v>52.597520803574284</v>
+      </c>
+      <c r="O3" s="4">
+        <f>(('Flat glass'!$D$19+O11))*$H$3</f>
+        <v>53.219755759253616</v>
+      </c>
+      <c r="P3" s="4">
+        <f>(('Flat glass'!$D$19+P11))*$H$3</f>
+        <v>53.219755759253616</v>
+      </c>
+      <c r="Q3" s="4">
+        <f>(('Flat glass'!$D$19+Q11))*$H$3</f>
+        <v>53.219755759253616</v>
+      </c>
+      <c r="S3" s="8">
+        <f t="shared" ref="S3:S27" si="0">N3/$D3</f>
+        <v>0.98830819595463593</v>
+      </c>
+      <c r="T3" s="8">
+        <f t="shared" ref="T3:T27" si="1">O3/$D3</f>
+        <v>1</v>
+      </c>
+      <c r="U3" s="8">
+        <f t="shared" ref="U3:U27" si="2">P3/$D3</f>
+        <v>1</v>
+      </c>
+      <c r="V3" s="8">
+        <f t="shared" ref="V3:V27" si="3">Q3/$D3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
         <v>72</v>
-      </c>
-      <c r="B4" t="s">
-        <v>73</v>
       </c>
       <c r="C4" t="s">
         <v>37</v>
       </c>
       <c r="D4" s="4">
-        <f>(('Flat glass'!D19+D12))*H2</f>
+        <f>(('Flat glass'!$D$19+D11))*$H$2</f>
         <v>11.788444010275478</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
       </c>
       <c r="G4" t="s">
         <v>38</v>
@@ -1296,29 +1469,119 @@
       <c r="H4" s="5">
         <v>0.84530000000000005</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D5" s="4"/>
+      <c r="I4" s="5">
+        <f>H4+I20</f>
+        <v>0.85530000000000006</v>
+      </c>
+      <c r="N4" s="4">
+        <f>(('Flat glass'!$D$19+N11))*$H$2</f>
+        <v>11.65061583290759</v>
+      </c>
+      <c r="O4" s="4">
+        <f>(('Flat glass'!$D$19+O11))*$H$2</f>
+        <v>11.788444010275478</v>
+      </c>
+      <c r="P4" s="4">
+        <f>(('Flat glass'!$D$19+P11))*$H$2</f>
+        <v>11.788444010275478</v>
+      </c>
+      <c r="Q4" s="4">
+        <f>(('Flat glass'!$D$19+Q11))*$H$2</f>
+        <v>11.788444010275478</v>
+      </c>
+      <c r="S4" s="8">
+        <f t="shared" si="0"/>
+        <v>0.98830819595463582</v>
+      </c>
+      <c r="T4" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U4" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V4" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="4">
+        <f>(('Container glass'!$D$13+D9)-(SUM(D20:D22)))*$H$1</f>
+        <v>13.58776385767761</v>
+      </c>
+      <c r="F5" t="s">
+        <v>88</v>
+      </c>
       <c r="G5" t="s">
         <v>39</v>
       </c>
       <c r="H5" s="5">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="5">
+        <f>H5-I20</f>
+        <v>9.0000000000000011E-2</v>
+      </c>
+      <c r="N5" s="4">
+        <f>(('Container glass'!$D$13+N9)-(SUM(N20:N22)))*$H$1</f>
+        <v>13.428898385238961</v>
+      </c>
+      <c r="O5" s="4">
+        <f>(('Container glass'!$D$13+O9)-(SUM(O20:O22)))*$H$1</f>
+        <v>13.58776385767761</v>
+      </c>
+      <c r="P5" s="4">
+        <f>(('Container glass'!$D$13+P9)-(SUM(P20:P22)))*$H$1</f>
+        <v>13.58776385767761</v>
+      </c>
+      <c r="Q5" s="4">
+        <f>(('Container glass'!$D$13+Q9)-(SUM(Q20:Q22)))*$H$1</f>
+        <v>13.378721336790262</v>
+      </c>
+      <c r="S5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.98830819595463582</v>
+      </c>
+      <c r="T5" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U5" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V5" s="8">
+        <f t="shared" si="3"/>
+        <v>0.98461538461538467</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6" s="4">
-        <f>(('Container glass'!D13+D10)-(SUM(D23:D25)))*H1</f>
-        <v>13.58776385767761</v>
+        <f>(('Container glass'!$D$13+D9)-(SUM(D20:D22)))*$H$3</f>
+        <v>38.513822411409272</v>
+      </c>
+      <c r="F6" t="s">
+        <v>89</v>
       </c>
       <c r="G6" t="s">
         <v>40</v>
@@ -1326,20 +1589,59 @@
       <c r="H6" s="5">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="5">
+        <f>H6-I20</f>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="N6" s="4">
+        <f>(('Container glass'!$D$13+N9)-(SUM(N20:N22)))*$H$3</f>
+        <v>38.06352634673712</v>
+      </c>
+      <c r="O6" s="4">
+        <f>(('Container glass'!$D$13+O9)-(SUM(O20:O22)))*$H$3</f>
+        <v>38.513822411409272</v>
+      </c>
+      <c r="P6" s="4">
+        <f>(('Container glass'!$D$13+P9)-(SUM(P20:P22)))*$H$3</f>
+        <v>38.513822411409272</v>
+      </c>
+      <c r="Q6" s="4">
+        <f>(('Container glass'!$D$13+Q9)-(SUM(Q20:Q22)))*$H$3</f>
+        <v>37.92130206661836</v>
+      </c>
+      <c r="S6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.98830819595463582</v>
+      </c>
+      <c r="T6" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U6" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V6" s="8">
+        <f t="shared" si="3"/>
+        <v>0.98461538461538456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D7" s="4">
-        <f>(('Container glass'!D13+D10)-(SUM(D23:D25)))*H3</f>
-        <v>38.513822411409272</v>
+        <f>(('Container glass'!$D$13+D9)-(SUM(D20:D22)))*$H$2</f>
+        <v>8.5310056884214163</v>
+      </c>
+      <c r="F7" t="s">
+        <v>90</v>
       </c>
       <c r="G7" t="s">
         <v>41</v>
@@ -1347,20 +1649,59 @@
       <c r="H7" s="5">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="5">
+        <f>H7+I20</f>
+        <v>0.76</v>
+      </c>
+      <c r="N7" s="4">
+        <f>(('Container glass'!$D$13+N9)-(SUM(N20:N22)))*$H$2</f>
+        <v>8.4312628416025071</v>
+      </c>
+      <c r="O7" s="4">
+        <f>(('Container glass'!$D$13+O9)-(SUM(O20:O22)))*$H$2</f>
+        <v>8.5310056884214163</v>
+      </c>
+      <c r="P7" s="4">
+        <f>(('Container glass'!$D$13+P9)-(SUM(P20:P22)))*$H$2</f>
+        <v>8.5310056884214163</v>
+      </c>
+      <c r="Q7" s="4">
+        <f>(('Container glass'!$D$13+Q9)-(SUM(Q20:Q22)))*$H$2</f>
+        <v>8.3997594470610881</v>
+      </c>
+      <c r="S7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.98830819595463593</v>
+      </c>
+      <c r="T7" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U7" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V7" s="8">
+        <f t="shared" si="3"/>
+        <v>0.98461538461538478</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
         <v>74</v>
       </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
       <c r="D8" s="4">
-        <f>(('Container glass'!D13+D10)-(SUM(D23:D25)))*H2</f>
-        <v>8.5310056884214163</v>
+        <f>SUM(D14:D16)/(1-$H$5)</f>
+        <v>87.61150424219106</v>
+      </c>
+      <c r="F8" t="s">
+        <v>91</v>
       </c>
       <c r="G8" t="s">
         <v>42</v>
@@ -1368,20 +1709,59 @@
       <c r="H8" s="5">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="7">
+        <f>H8-I20/2</f>
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="N8" s="4">
+        <f>SUM(N14:N16)/(1-$H$5)</f>
+        <v>87.61150424219106</v>
+      </c>
+      <c r="O8" s="4">
+        <f>SUM(O14:O16)/(1-$I$5)</f>
+        <v>86.648740459309835</v>
+      </c>
+      <c r="P8" s="4">
+        <f>SUM(P14:P16)/(1-$H$5)</f>
+        <v>87.61150424219106</v>
+      </c>
+      <c r="Q8" s="4">
+        <f>SUM(Q14:Q16)/(1-$H$5)</f>
+        <v>87.61150424219106</v>
+      </c>
+      <c r="S8" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T8" s="8">
+        <f t="shared" si="1"/>
+        <v>0.98901098901098894</v>
+      </c>
+      <c r="U8" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V8" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
         <v>75</v>
       </c>
       <c r="D9" s="4">
-        <f>SUM(D17:D19)/(1-H5)</f>
-        <v>87.61150424219106</v>
+        <f>(('Container glass'!$D$13-SUM(D20:D22))/$H$4)*(1-$H$4)</f>
+        <v>9.3798619758265307</v>
+      </c>
+      <c r="F9" t="s">
+        <v>92</v>
       </c>
       <c r="G9" t="s">
         <v>43</v>
@@ -1389,20 +1769,59 @@
       <c r="H9" s="5">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="7">
+        <f>H9-I20/2</f>
+        <v>4.5000000000000005E-2</v>
+      </c>
+      <c r="N9" s="4">
+        <f>(('Container glass'!$D$13-SUM(N20:N22))/$I$4)*(1-$I$4)</f>
+        <v>8.6709575918968174</v>
+      </c>
+      <c r="O9" s="4">
+        <f>(('Container glass'!$D$13-SUM(O20:O22))/$H$4)*(1-$H$4)</f>
+        <v>9.3798619758265307</v>
+      </c>
+      <c r="P9" s="4">
+        <f>(('Container glass'!$D$13-SUM(P20:P22))/$H$4)*(1-$H$4)</f>
+        <v>9.3798619758265307</v>
+      </c>
+      <c r="Q9" s="4">
+        <f>(('Container glass'!$D$13-SUM(Q20:Q22))/$H$4)*(1-$H$4)</f>
+        <v>9.2355564069676603</v>
+      </c>
+      <c r="S9" s="8">
+        <f t="shared" si="0"/>
+        <v>0.92442272756713495</v>
+      </c>
+      <c r="T9" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U9" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V9" s="8">
+        <f t="shared" si="3"/>
+        <v>0.98461538461538456</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
         <v>74</v>
       </c>
-      <c r="B10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" t="s">
-        <v>76</v>
-      </c>
       <c r="D10" s="4">
-        <f>(('Container glass'!D13-SUM(D23:D25))/H4)*(1-H4)</f>
-        <v>9.3798619758265307</v>
+        <f>'Flat glass'!$D$19/(1-$H$6)</f>
+        <v>83.320972631680775</v>
+      </c>
+      <c r="F10" t="s">
+        <v>93</v>
       </c>
       <c r="G10" t="s">
         <v>44</v>
@@ -1410,20 +1829,59 @@
       <c r="H10" s="5">
         <v>0.83</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="5">
+        <f>H10+I20</f>
+        <v>0.84</v>
+      </c>
+      <c r="N10" s="4">
+        <f>'Flat glass'!$D$19/(1-$H$6)</f>
+        <v>83.320972631680775</v>
+      </c>
+      <c r="O10" s="4">
+        <f>'Flat glass'!$D$19/(1-$I$6)</f>
+        <v>82.352124112707742</v>
+      </c>
+      <c r="P10" s="4">
+        <f>'Flat glass'!$D$19/(1-$H$6)</f>
+        <v>83.320972631680775</v>
+      </c>
+      <c r="Q10" s="4">
+        <f>'Flat glass'!$D$19/(1-$H$6)</f>
+        <v>83.320972631680775</v>
+      </c>
+      <c r="S10" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T10" s="8">
+        <f t="shared" si="1"/>
+        <v>0.98837209302325579</v>
+      </c>
+      <c r="U10" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V10" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
         <v>75</v>
       </c>
       <c r="D11" s="4">
-        <f>'Flat glass'!D19/(1-H6)</f>
-        <v>83.320972631680775</v>
+        <f>('Flat glass'!$D$19/$H$4)*(1-$H$4)</f>
+        <v>12.961423513785473</v>
+      </c>
+      <c r="F11" t="s">
+        <v>94</v>
       </c>
       <c r="G11" t="s">
         <v>45</v>
@@ -1431,20 +1889,59 @@
       <c r="H11" s="5">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="7">
+        <f>H11-I20/2</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="N11" s="4">
+        <f>('Flat glass'!$D$19/$I$4)*(1-$I$4)</f>
+        <v>11.981834477766366</v>
+      </c>
+      <c r="O11" s="4">
+        <f>('Flat glass'!$D$19/$H$4)*(1-$H$4)</f>
+        <v>12.961423513785473</v>
+      </c>
+      <c r="P11" s="4">
+        <f>('Flat glass'!$D$19/$H$4)*(1-$H$4)</f>
+        <v>12.961423513785473</v>
+      </c>
+      <c r="Q11" s="4">
+        <f>('Flat glass'!$D$19/$H$4)*(1-$H$4)</f>
+        <v>12.961423513785473</v>
+      </c>
+      <c r="S11" s="8">
+        <f t="shared" si="0"/>
+        <v>0.92442272756713506</v>
+      </c>
+      <c r="T11" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U11" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V11" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" t="s">
         <v>73</v>
       </c>
-      <c r="B12" t="s">
-        <v>67</v>
-      </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D12" s="4">
-        <f>('Flat glass'!D19/H4)*(1-H4)</f>
-        <v>12.961423513785473</v>
+        <f>(SUM(D14:D16)/(1-$H$5))-SUM(D14:D16)</f>
+        <v>8.7611504242191103</v>
+      </c>
+      <c r="F12" t="s">
+        <v>95</v>
       </c>
       <c r="G12" t="s">
         <v>46</v>
@@ -1452,287 +1949,1152 @@
       <c r="H12" s="5">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="4"/>
+      <c r="I12" s="7">
+        <f>H12-I20/2</f>
+        <v>0.105</v>
+      </c>
+      <c r="N12" s="4">
+        <f>(SUM(N14:N16)/(1-$H$5))-SUM(N14:N16)</f>
+        <v>8.7611504242191103</v>
+      </c>
+      <c r="O12" s="4">
+        <f>(SUM(O14:O16)/(1-$I$5))-SUM(O14:O16)</f>
+        <v>7.7983866413378848</v>
+      </c>
+      <c r="P12" s="4">
+        <f>(SUM(P14:P16)/(1-$H$5))-SUM(P14:P16)</f>
+        <v>8.7611504242191103</v>
+      </c>
+      <c r="Q12" s="4">
+        <f>(SUM(Q14:Q16)/(1-$H$5))-SUM(Q14:Q16)</f>
+        <v>8.7611504242191103</v>
+      </c>
+      <c r="S12" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T12" s="8">
+        <f t="shared" si="1"/>
+        <v>0.89010989010988961</v>
+      </c>
+      <c r="U12" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V12" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="4">
+        <f>('Flat glass'!$D$19/(1-$H$6))-'Flat glass'!$D$19</f>
+        <v>12.498145894752113</v>
+      </c>
+      <c r="F13" t="s">
+        <v>96</v>
+      </c>
       <c r="G13" t="s">
         <v>47</v>
       </c>
       <c r="H13" s="6">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="4"/>
-      <c r="G14" t="s">
+      <c r="I13" s="6">
+        <f>H13+I20</f>
+        <v>0.36</v>
+      </c>
+      <c r="N13" s="4">
+        <f>('Flat glass'!$D$19/(1-$H$6))-'Flat glass'!$D$19</f>
+        <v>12.498145894752113</v>
+      </c>
+      <c r="O13" s="4">
+        <f>('Flat glass'!$D$19/(1-$I$6))-'Flat glass'!$D$19</f>
+        <v>11.52929737577908</v>
+      </c>
+      <c r="P13" s="4">
+        <f>('Flat glass'!$D$19/(1-$H$6))-'Flat glass'!$D$19</f>
+        <v>12.498145894752113</v>
+      </c>
+      <c r="Q13" s="4">
+        <f>('Flat glass'!$D$19/(1-$H$6))-'Flat glass'!$D$19</f>
+        <v>12.498145894752113</v>
+      </c>
+      <c r="S13" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T13" s="8">
+        <f t="shared" si="1"/>
+        <v>0.92248062015503873</v>
+      </c>
+      <c r="U13" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V13" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="4">
+        <f>'Container glass'!$D$13*$H$7</f>
+        <v>59.137765363478962</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="N14" s="4">
+        <f>'Container glass'!$D$13*$H$7</f>
+        <v>59.137765363478962</v>
+      </c>
+      <c r="O14" s="4">
+        <f>'Container glass'!$D$13*$H$7</f>
+        <v>59.137765363478962</v>
+      </c>
+      <c r="P14" s="4">
+        <f>'Container glass'!$D$13*$I$7</f>
+        <v>59.92626890165868</v>
+      </c>
+      <c r="Q14" s="4">
+        <f>'Container glass'!$D$13*$H$7</f>
+        <v>59.137765363478962</v>
+      </c>
+      <c r="S14" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T14" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U14" s="8">
+        <f t="shared" si="2"/>
+        <v>1.0133333333333334</v>
+      </c>
+      <c r="V14" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="4">
+        <f>'Container glass'!$D$13*$H$8</f>
+        <v>15.77007076359439</v>
+      </c>
+      <c r="N15" s="4">
+        <f>'Container glass'!$D$13*$H$8</f>
+        <v>15.77007076359439</v>
+      </c>
+      <c r="O15" s="4">
+        <f>'Container glass'!$D$13*$H$8</f>
+        <v>15.77007076359439</v>
+      </c>
+      <c r="P15" s="4">
+        <f>'Container glass'!$D$13*$I$8</f>
+        <v>15.375818994504531</v>
+      </c>
+      <c r="Q15" s="4">
+        <f>'Container glass'!$D$13*$H$8</f>
+        <v>15.77007076359439</v>
+      </c>
+      <c r="S15" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T15" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U15" s="8">
+        <f t="shared" si="2"/>
+        <v>0.97500000000000009</v>
+      </c>
+      <c r="V15" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="4">
+        <f>'Container glass'!$D$13*$H$9</f>
+        <v>3.9425176908985975</v>
+      </c>
+      <c r="G16" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="6">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" s="4">
-        <f>(SUM(D17:D19)/(1-H5))-SUM(D17:D19)</f>
-        <v>8.7611504242191103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" s="4">
-        <f>('Flat glass'!D19/(1-H6))-'Flat glass'!D19</f>
-        <v>12.498145894752113</v>
-      </c>
-      <c r="G16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N16" s="4">
+        <f>'Container glass'!$D$13*$H$9</f>
+        <v>3.9425176908985975</v>
+      </c>
+      <c r="O16" s="4">
+        <f>'Container glass'!$D$13*$H$9</f>
+        <v>3.9425176908985975</v>
+      </c>
+      <c r="P16" s="4">
+        <f>'Container glass'!$D$13*$I$9</f>
+        <v>3.548265921808738</v>
+      </c>
+      <c r="Q16" s="4">
+        <f>'Container glass'!$D$13*$H$9</f>
+        <v>3.9425176908985975</v>
+      </c>
+      <c r="S16" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T16" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U16" s="8">
+        <f>P16/$D16</f>
+        <v>0.9</v>
+      </c>
+      <c r="V16" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="4">
+        <f>'Flat glass'!$D$19*$H$10</f>
+        <v>58.782946191650787</v>
+      </c>
+      <c r="G17" t="s">
         <v>50</v>
-      </c>
-      <c r="D17" s="4">
-        <f>'Container glass'!D13*H7</f>
-        <v>59.137765363478962</v>
-      </c>
-      <c r="G17" t="s">
-        <v>51</v>
       </c>
       <c r="H17" s="5">
         <v>0.37490000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N17" s="4">
+        <f>'Flat glass'!$D$19*$H$10</f>
+        <v>58.782946191650787</v>
+      </c>
+      <c r="O17" s="4">
+        <f>'Flat glass'!$D$19*$H$10</f>
+        <v>58.782946191650787</v>
+      </c>
+      <c r="P17" s="4">
+        <f>'Flat glass'!$D$19*$I$10</f>
+        <v>59.491174459020073</v>
+      </c>
+      <c r="Q17" s="4">
+        <f>'Flat glass'!$D$19*$H$10</f>
+        <v>58.782946191650787</v>
+      </c>
+      <c r="S17" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T17" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U17" s="8">
+        <f t="shared" si="2"/>
+        <v>1.0120481927710843</v>
+      </c>
+      <c r="V17" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="4">
+        <f>'Flat glass'!$D$19*$H$11</f>
+        <v>4.2493696042157199</v>
+      </c>
+      <c r="G18" t="s">
         <v>52</v>
-      </c>
-      <c r="D18" s="4">
-        <f>'Container glass'!D13*H8</f>
-        <v>15.77007076359439</v>
-      </c>
-      <c r="G18" t="s">
-        <v>53</v>
       </c>
       <c r="H18" s="5">
         <v>0.1298</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N18" s="4">
+        <f>'Flat glass'!$D$19*$H$11</f>
+        <v>4.2493696042157199</v>
+      </c>
+      <c r="O18" s="4">
+        <f>'Flat glass'!$D$19*$H$11</f>
+        <v>4.2493696042157199</v>
+      </c>
+      <c r="P18" s="4">
+        <f>'Flat glass'!$D$19*$I$11</f>
+        <v>3.8952554705310765</v>
+      </c>
+      <c r="Q18" s="4">
+        <f>'Flat glass'!$D$19*$H$11</f>
+        <v>4.2493696042157199</v>
+      </c>
+      <c r="S18" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T18" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U18" s="8">
+        <f t="shared" si="2"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="V18" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D19" s="4">
-        <f>'Container glass'!D13*H9</f>
-        <v>3.9425176908985975</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <f>'Flat glass'!$D$19*$H$12</f>
+        <v>7.7905109410621529</v>
+      </c>
+      <c r="N19" s="4">
+        <f>'Flat glass'!$D$19*$H$12</f>
+        <v>7.7905109410621529</v>
+      </c>
+      <c r="O19" s="4">
+        <f>'Flat glass'!$D$19*$H$12</f>
+        <v>7.7905109410621529</v>
+      </c>
+      <c r="P19" s="4">
+        <f>'Flat glass'!$D$19*$I$12</f>
+        <v>7.4363968073775091</v>
+      </c>
+      <c r="Q19" s="4">
+        <f>'Flat glass'!$D$19*$H$12</f>
+        <v>7.7905109410621529</v>
+      </c>
+      <c r="S19" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T19" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U19" s="8">
+        <f t="shared" si="2"/>
+        <v>0.95454545454545447</v>
+      </c>
+      <c r="V19" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D20" s="4">
-        <f>'Flat glass'!D19*H10</f>
-        <v>58.782946191650787</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <f>D14*$H$13</f>
+        <v>20.698217877217637</v>
+      </c>
+      <c r="H20" t="s">
+        <v>85</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="N20" s="4">
+        <f>N14*$H$13</f>
+        <v>20.698217877217637</v>
+      </c>
+      <c r="O20" s="4">
+        <f>O14*$H$13</f>
+        <v>20.698217877217637</v>
+      </c>
+      <c r="P20" s="4">
+        <f>P14*$H$13</f>
+        <v>20.974194115580538</v>
+      </c>
+      <c r="Q20" s="4">
+        <f>Q14*$I$13</f>
+        <v>21.289595530852427</v>
+      </c>
+      <c r="S20" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T20" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U20" s="8">
+        <f t="shared" si="2"/>
+        <v>1.0133333333333332</v>
+      </c>
+      <c r="V20" s="8">
+        <f t="shared" si="3"/>
+        <v>1.0285714285714287</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D21" s="4">
-        <f>'Flat glass'!D19*H11</f>
-        <v>4.2493696042157199</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <f>D15*$H$13</f>
+        <v>5.5195247672580363</v>
+      </c>
+      <c r="N21" s="4">
+        <f>N15*$H$13</f>
+        <v>5.5195247672580363</v>
+      </c>
+      <c r="O21" s="4">
+        <f>O15*$H$13</f>
+        <v>5.5195247672580363</v>
+      </c>
+      <c r="P21" s="4">
+        <f>P15*$H$13</f>
+        <v>5.3815366480765858</v>
+      </c>
+      <c r="Q21" s="4">
+        <f>Q15*$I$13</f>
+        <v>5.6772254748939801</v>
+      </c>
+      <c r="S21" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T21" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U21" s="8">
+        <f t="shared" si="2"/>
+        <v>0.97500000000000009</v>
+      </c>
+      <c r="V21" s="8">
+        <f t="shared" si="3"/>
+        <v>1.0285714285714285</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>78</v>
       </c>
       <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="4">
+        <f>D16*$H$13</f>
+        <v>1.3798811918145091</v>
+      </c>
+      <c r="N22" s="4">
+        <f>N16*$H$13</f>
+        <v>1.3798811918145091</v>
+      </c>
+      <c r="O22" s="4">
+        <f>O16*$H$13</f>
+        <v>1.3798811918145091</v>
+      </c>
+      <c r="P22" s="4">
+        <f>P16*$H$13</f>
+        <v>1.2418930726330581</v>
+      </c>
+      <c r="Q22" s="4">
+        <f>Q16*$I$13</f>
+        <v>1.419306368723495</v>
+      </c>
+      <c r="S22" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T22" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U22" s="8">
+        <f t="shared" si="2"/>
+        <v>0.9</v>
+      </c>
+      <c r="V22" s="8">
+        <f t="shared" si="3"/>
+        <v>1.0285714285714285</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
         <v>81</v>
       </c>
-      <c r="C22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="4">
-        <f>'Flat glass'!D19*H12</f>
-        <v>7.7905109410621529</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" t="s">
-        <v>74</v>
-      </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="4">
-        <f>D17*H13</f>
-        <v>20.698217877217637</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <f>D14*(1-$H$13)</f>
+        <v>38.439547486261326</v>
+      </c>
+      <c r="N23" s="4">
+        <f>N14*(1-$H$13)</f>
+        <v>38.439547486261326</v>
+      </c>
+      <c r="O23" s="4">
+        <f>O14*(1-$H$13)</f>
+        <v>38.439547486261326</v>
+      </c>
+      <c r="P23" s="4">
+        <f>P14*(1-$H$13)</f>
+        <v>38.952074786078143</v>
+      </c>
+      <c r="Q23" s="4">
+        <f>Q14*(1-$I$13)</f>
+        <v>37.848169832626539</v>
+      </c>
+      <c r="S23" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T23" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U23" s="8">
+        <f t="shared" si="2"/>
+        <v>1.0133333333333334</v>
+      </c>
+      <c r="V23" s="8">
+        <f t="shared" si="3"/>
+        <v>0.98461538461538467</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" s="4">
-        <f>D18*H13</f>
-        <v>5.5195247672580363</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <f>D15*(1-$H$13)</f>
+        <v>10.250545996336355</v>
+      </c>
+      <c r="N24" s="4">
+        <f>N15*(1-$H$13)</f>
+        <v>10.250545996336355</v>
+      </c>
+      <c r="O24" s="4">
+        <f>O15*(1-$H$13)</f>
+        <v>10.250545996336355</v>
+      </c>
+      <c r="P24" s="4">
+        <f>P15*(1-$H$13)</f>
+        <v>9.994282346427946</v>
+      </c>
+      <c r="Q24" s="4">
+        <f>Q15*(1-$I$13)</f>
+        <v>10.09284528870041</v>
+      </c>
+      <c r="S24" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T24" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U24" s="8">
+        <f t="shared" si="2"/>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="V24" s="8">
+        <f t="shared" si="3"/>
+        <v>0.98461538461538456</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="4">
+        <f>D16*(1-$H$13)</f>
+        <v>2.5626364990840886</v>
+      </c>
+      <c r="N25" s="4">
+        <f>N16*(1-$H$13)</f>
+        <v>2.5626364990840886</v>
+      </c>
+      <c r="O25" s="4">
+        <f>O16*(1-$H$13)</f>
+        <v>2.5626364990840886</v>
+      </c>
+      <c r="P25" s="4">
+        <f>P16*(1-$H$13)</f>
+        <v>2.3063728491756796</v>
+      </c>
+      <c r="Q25" s="4">
+        <f>Q16*(1-$I$13)</f>
+        <v>2.5232113221751025</v>
+      </c>
+      <c r="S25" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T25" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U25" s="8">
+        <f t="shared" si="2"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="V25" s="8">
+        <f t="shared" si="3"/>
+        <v>0.98461538461538456</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="4">
-        <f>D19*H13</f>
-        <v>1.3798811918145091</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" t="s">
-        <v>50</v>
-      </c>
       <c r="D26" s="4">
-        <f>D17*H14</f>
-        <v>38.439547486261326</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="4">
-        <f>D18*H14</f>
-        <v>10.250545996336355</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="4">
-        <f>D19*H14</f>
-        <v>2.5626364990840886</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="4">
         <f>4.3+2.7+12.5+0.4+0.4+0.1</f>
         <v>20.399999999999999</v>
       </c>
-      <c r="E29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="E26" t="s">
+        <v>57</v>
+      </c>
+      <c r="N26" s="4">
+        <f>4.3+2.7+12.5+0.4+0.4+0.1</f>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="O26" s="4">
+        <f>4.3+2.7+12.5+0.4+0.4+0.1</f>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="P26" s="4">
+        <f>4.3+2.7+12.5+0.4+0.4+0.1</f>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="Q26" s="4">
+        <f>4.3+2.7+12.5+0.4+0.4+0.1</f>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="S26" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T26" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U26" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V26" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" t="s">
         <v>81</v>
       </c>
-      <c r="B30" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="4">
+      <c r="C27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="4">
         <f>(0.15+0.25+0.08+0.1)*100/(15+16+16+28)</f>
         <v>0.77333333333333343</v>
       </c>
-      <c r="E30" t="s">
-        <v>59</v>
+      <c r="E27" t="s">
+        <v>58</v>
+      </c>
+      <c r="N27" s="4">
+        <f>(0.15+0.25+0.08+0.1)*100/(15+16+16+28)</f>
+        <v>0.77333333333333343</v>
+      </c>
+      <c r="O27" s="4">
+        <f>(0.15+0.25+0.08+0.1)*100/(15+16+16+28)</f>
+        <v>0.77333333333333343</v>
+      </c>
+      <c r="P27" s="4">
+        <f>(0.15+0.25+0.08+0.1)*100/(15+16+16+28)</f>
+        <v>0.77333333333333343</v>
+      </c>
+      <c r="Q27" s="4">
+        <f>(0.15+0.25+0.08+0.1)*100/(15+16+16+28)</f>
+        <v>0.77333333333333343</v>
+      </c>
+      <c r="S27" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T27" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U27" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V27" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="X30" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="X31" t="str">
+        <f>A9</f>
+        <v>CGM</v>
+      </c>
+      <c r="Y31" t="str">
+        <f>B9</f>
+        <v>loss1</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB31" s="9">
+        <f>S9</f>
+        <v>0.92442272756713495</v>
+      </c>
+      <c r="AC31" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD31" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE31" s="9">
+        <f>V9</f>
+        <v>0.98461538461538456</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="X32" t="str">
+        <f>A11</f>
+        <v>FGM</v>
+      </c>
+      <c r="Y32" t="str">
+        <f>B11</f>
+        <v>loss2</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB32" s="9">
+        <f>S11</f>
+        <v>0.92442272756713506</v>
+      </c>
+      <c r="AC32" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD32" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE32" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="24:31" x14ac:dyDescent="0.25">
+      <c r="X33" t="str">
+        <f>A12</f>
+        <v>CGF</v>
+      </c>
+      <c r="Y33" t="str">
+        <f>B12</f>
+        <v>CGM</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB33" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC33" s="9">
+        <f>T12</f>
+        <v>0.89010989010988961</v>
+      </c>
+      <c r="AD33" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE33" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="24:31" x14ac:dyDescent="0.25">
+      <c r="X34" t="str">
+        <f>A13</f>
+        <v>FGF</v>
+      </c>
+      <c r="Y34" t="str">
+        <f>B13</f>
+        <v>FGM</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB34" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC34" s="9">
+        <f>T13</f>
+        <v>0.92248062015503873</v>
+      </c>
+      <c r="AD34" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE34" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="24:31" x14ac:dyDescent="0.25">
+      <c r="X35" t="str">
+        <f>A16</f>
+        <v>CGF</v>
+      </c>
+      <c r="Y35" t="str">
+        <f>B16</f>
+        <v>CGU</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB35" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC35" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD35" s="9">
+        <f>U16</f>
+        <v>0.9</v>
+      </c>
+      <c r="AE35" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="24:31" x14ac:dyDescent="0.25">
+      <c r="X36" t="str">
+        <f>A18</f>
+        <v>FGF</v>
+      </c>
+      <c r="Y36" t="str">
+        <f>B18</f>
+        <v>FGU</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB36" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC36" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD36" s="9">
+        <f>U18</f>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="AE36" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="24:31" x14ac:dyDescent="0.25">
+      <c r="X37" t="str">
+        <f>A19</f>
+        <v>FGF</v>
+      </c>
+      <c r="Y37" t="str">
+        <f>B19</f>
+        <v>FGU</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB37" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC37" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD37" s="9">
+        <f>U19</f>
+        <v>0.95454545454545447</v>
+      </c>
+      <c r="AE37" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="24:31" x14ac:dyDescent="0.25">
+      <c r="X38" t="str">
+        <f>A20</f>
+        <v>CGU</v>
+      </c>
+      <c r="Y38" t="str">
+        <f>B20</f>
+        <v>CGM</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB38" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC38" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD38" s="9">
+        <f>U20</f>
+        <v>1.0133333333333332</v>
+      </c>
+      <c r="AE38" s="9">
+        <f>V20</f>
+        <v>1.0285714285714287</v>
+      </c>
+    </row>
+    <row r="39" spans="24:31" x14ac:dyDescent="0.25">
+      <c r="X39" t="str">
+        <f>A21</f>
+        <v>CGU</v>
+      </c>
+      <c r="Y39" t="str">
+        <f>B21</f>
+        <v>CGM</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB39" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC39" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD39" s="9">
+        <f>U21</f>
+        <v>0.97500000000000009</v>
+      </c>
+      <c r="AE39" s="9">
+        <f>V21</f>
+        <v>1.0285714285714285</v>
+      </c>
+    </row>
+    <row r="40" spans="24:31" x14ac:dyDescent="0.25">
+      <c r="X40" t="str">
+        <f>A22</f>
+        <v>CGU</v>
+      </c>
+      <c r="Y40" t="str">
+        <f>B22</f>
+        <v>CGM</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB40" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC40" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD40" s="9">
+        <f>U22</f>
+        <v>0.9</v>
+      </c>
+      <c r="AE40" s="9">
+        <f>V22</f>
+        <v>1.0285714285714285</v>
+      </c>
+    </row>
+    <row r="41" spans="24:31" x14ac:dyDescent="0.25">
+      <c r="X41" t="str">
+        <f>A25</f>
+        <v>CGU</v>
+      </c>
+      <c r="Y41" t="str">
+        <f>B25</f>
+        <v>EoL</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB41" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC41" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD41" s="9">
+        <f>U25</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="AE41" s="9">
+        <f>V25</f>
+        <v>0.98461538461538456</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="S2:V27">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added stock model of glass in buildings
</commit_message>
<xml_diff>
--- a/data/glass_paper.xlsx
+++ b/data/glass_paper.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Desktop\python\glass-paper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D457E642-3813-4F98-9106-A06B99EB67CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350917CF-10AA-463C-B610-EB2A7DE5ED26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-5925" windowWidth="30960" windowHeight="16920" activeTab="3" xr2:uid="{1AC0E601-1297-4C8D-8E5F-6A8C787FDED8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{1AC0E601-1297-4C8D-8E5F-6A8C787FDED8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Container glass" sheetId="4" r:id="rId2"/>
     <sheet name="Flat glass" sheetId="2" r:id="rId3"/>
     <sheet name="Flows" sheetId="3" r:id="rId4"/>
+    <sheet name="Building_flows" sheetId="5" r:id="rId5"/>
+    <sheet name="Car_flows" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="110">
   <si>
     <t>Global production of glass</t>
   </si>
@@ -83,9 +85,6 @@
     <t>https://www.sciencedirect.com/science/article/pii/B9780128150603000153</t>
   </si>
   <si>
-    <t>Butler and Hooper, 2011</t>
-  </si>
-  <si>
     <t>National Bureau of Statistics of China, 2015</t>
   </si>
   <si>
@@ -116,9 +115,6 @@
     <t>Glass Alliance Europe, 2017</t>
   </si>
   <si>
-    <t>Pilkington 2010</t>
-  </si>
-  <si>
     <t>Other data available: https://www.wko.at/branchen/industrie/glasindustrie/statistical-report-glass-alliance-europe-2018-2019.pdf</t>
   </si>
   <si>
@@ -182,21 +178,12 @@
     <t>Global Cont Recycling Rate</t>
   </si>
   <si>
-    <t>%Cullet in Batch</t>
-  </si>
-  <si>
     <t>Beverages</t>
   </si>
   <si>
-    <t>Container</t>
-  </si>
-  <si>
     <t>Food</t>
   </si>
   <si>
-    <t>Flat</t>
-  </si>
-  <si>
     <t>Other CG</t>
   </si>
   <si>
@@ -209,9 +196,6 @@
     <t>Other FG</t>
   </si>
   <si>
-    <t>Table 15.6: https://www.sciencedirect.com/science/article/pii/B9780128150603000153</t>
-  </si>
-  <si>
     <t>Table 15.7: https://www.sciencedirect.com/science/article/pii/B9780128150603000153</t>
   </si>
   <si>
@@ -293,9 +277,6 @@
     <t>beta</t>
   </si>
   <si>
-    <t>variation</t>
-  </si>
-  <si>
     <t>gamma</t>
   </si>
   <si>
@@ -360,6 +341,33 @@
   </si>
   <si>
     <t>Disposal</t>
+  </si>
+  <si>
+    <t>Table 15.6 and table 15.7: https://www.sciencedirect.com/science/article/pii/B9780128150603000153</t>
+  </si>
+  <si>
+    <t>Sensitivity variation</t>
+  </si>
+  <si>
+    <t>Pilkington, 2010</t>
+  </si>
+  <si>
+    <t>Glabal flat glass construction and demolition waste [Mt]</t>
+  </si>
+  <si>
+    <t>Glabal flat glass automotive waste [Mt]</t>
+  </si>
+  <si>
+    <t>Out</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/B9780123814753100117</t>
+  </si>
+  <si>
+    <t>Table 11.7: https://www.sciencedirect.com/science/article/pii/B9780123814753100117</t>
   </si>
 </sst>
 </file>
@@ -370,7 +378,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,6 +395,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -416,7 +432,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -427,6 +443,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -746,7 +765,7 @@
   <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,7 +864,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -853,7 +872,7 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C3">
         <v>2014</v>
@@ -862,12 +881,12 @@
         <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C4">
         <v>2007</v>
@@ -876,12 +895,12 @@
         <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C5">
         <v>2007</v>
@@ -891,12 +910,12 @@
         <v>39851</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C6">
         <v>2014</v>
@@ -906,12 +925,12 @@
         <v>44959</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C7">
         <v>2014</v>
@@ -921,12 +940,12 @@
         <v>80.700707635943886</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C8">
         <v>2007</v>
@@ -935,12 +954,12 @@
         <v>4.2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C9">
         <v>2014</v>
@@ -949,12 +968,12 @@
         <v>4</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C10">
         <v>2007</v>
@@ -963,12 +982,12 @@
         <v>0.7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C11">
         <v>2014</v>
@@ -977,12 +996,12 @@
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C13">
         <v>2014</v>
@@ -992,7 +1011,7 @@
         <v>78.85035381797195</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1010,16 +1029,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EC93BF-3E27-439B-9576-A211E3A0EC5A}">
-  <dimension ref="B2:F19"/>
+  <dimension ref="B2:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
@@ -1030,7 +1049,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -1038,7 +1057,7 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>2014</v>
@@ -1055,7 +1074,7 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>2015</v>
@@ -1069,7 +1088,7 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>2006</v>
@@ -1078,12 +1097,12 @@
         <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>2014</v>
@@ -1092,12 +1111,12 @@
         <v>41.56</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>2014</v>
@@ -1106,12 +1125,12 @@
         <v>9.2799999999999994</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>2014</v>
@@ -1120,12 +1139,12 @@
         <v>3.53</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>2006</v>
@@ -1134,12 +1153,12 @@
         <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>2006</v>
@@ -1148,12 +1167,12 @@
         <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11">
         <v>2006</v>
@@ -1162,12 +1181,12 @@
         <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>2014</v>
@@ -1177,12 +1196,12 @@
         <v>75.513888888888886</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>2010</v>
@@ -1191,12 +1210,12 @@
         <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>2018</v>
@@ -1205,12 +1224,12 @@
         <v>10.6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15">
         <v>2010</v>
@@ -1220,12 +1239,12 @@
         <v>87208</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16">
         <v>2014</v>
@@ -1235,12 +1254,12 @@
         <v>116204</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="4">
         <v>2014</v>
@@ -1250,22 +1269,82 @@
         <v>71.95459132189707</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="10">
+        <v>2014</v>
+      </c>
+      <c r="D18" s="11">
+        <f>AVERAGE(D12,D3,D17)</f>
+        <v>70.822826736928661</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="C19">
+        <v>2006</v>
+      </c>
+      <c r="D19" s="2">
+        <f>0.9 + 0.59 + 0.85 + 0.15 + 0.14 + 0.06</f>
+        <v>2.69</v>
+      </c>
+      <c r="E19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20">
         <v>2014</v>
       </c>
-      <c r="D19" s="2">
-        <f>AVERAGE(D12,D3,D17)</f>
-        <v>70.822826736928661</v>
-      </c>
-      <c r="E19" t="s">
-        <v>30</v>
+      <c r="D20" s="2">
+        <f>2.6 + 1.6 + 0.2 + 7.5 + 0.4 + 0.1</f>
+        <v>12.4</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21">
+        <v>2014</v>
+      </c>
+      <c r="D21" s="2">
+        <f>(0.15+0.25+0.08+0.1)*100/(15+16+16+28)</f>
+        <v>0.77333333333333343</v>
+      </c>
+      <c r="E21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22">
+        <v>2006</v>
+      </c>
+      <c r="D22">
+        <f>0.01 + 0.04 + 0.08 + 0.1</f>
+        <v>0.23</v>
+      </c>
+      <c r="E22" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1285,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11B3549B-C2AB-4D75-AB88-A04A3C1A4639}">
   <dimension ref="A1:AE41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z44" sqref="Z44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,82 +1377,82 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H1" s="5">
         <v>0.22409999999999999</v>
       </c>
       <c r="N1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="O1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="P1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="Q1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="S1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="T1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="U1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="V1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" s="4">
-        <f>(('Flat glass'!$D$19+D11))*$H$1</f>
+        <f>(('Flat glass'!$D$18+D11))*$H$1</f>
         <v>18.776050481185038</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H2" s="5">
         <v>0.14069999999999999</v>
       </c>
       <c r="N2" s="4">
-        <f>(('Flat glass'!$D$19+N11))*$H$1</f>
+        <f>(('Flat glass'!$D$18+N11))*$H$1</f>
         <v>18.556524578213157</v>
       </c>
       <c r="O2" s="4">
-        <f>(('Flat glass'!$D$19+O11))*$H$1</f>
+        <f>(('Flat glass'!$D$18+O11))*$H$1</f>
         <v>18.776050481185038</v>
       </c>
       <c r="P2" s="4">
-        <f>(('Flat glass'!$D$19+P11))*$H$1</f>
+        <f>(('Flat glass'!$D$18+P11))*$H$1</f>
         <v>18.776050481185038</v>
       </c>
       <c r="Q2" s="4">
-        <f>(('Flat glass'!$D$19+Q11))*$H$1</f>
+        <f>(('Flat glass'!$D$18+Q11))*$H$1</f>
         <v>18.776050481185038</v>
       </c>
       <c r="S2" s="8">
@@ -1395,38 +1474,38 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="4">
-        <f>(('Flat glass'!$D$19+D11))*$H$3</f>
+        <f>(('Flat glass'!$D$18+D11))*$H$3</f>
         <v>53.219755759253616</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H3" s="5">
         <v>0.63519999999999999</v>
       </c>
       <c r="N3" s="4">
-        <f>(('Flat glass'!$D$19+N11))*$H$3</f>
+        <f>(('Flat glass'!$D$18+N11))*$H$3</f>
         <v>52.597520803574284</v>
       </c>
       <c r="O3" s="4">
-        <f>(('Flat glass'!$D$19+O11))*$H$3</f>
+        <f>(('Flat glass'!$D$18+O11))*$H$3</f>
         <v>53.219755759253616</v>
       </c>
       <c r="P3" s="4">
-        <f>(('Flat glass'!$D$19+P11))*$H$3</f>
+        <f>(('Flat glass'!$D$18+P11))*$H$3</f>
         <v>53.219755759253616</v>
       </c>
       <c r="Q3" s="4">
-        <f>(('Flat glass'!$D$19+Q11))*$H$3</f>
+        <f>(('Flat glass'!$D$18+Q11))*$H$3</f>
         <v>53.219755759253616</v>
       </c>
       <c r="S3" s="8">
@@ -1448,45 +1527,45 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" s="4">
-        <f>(('Flat glass'!$D$19+D11))*$H$2</f>
+        <f>(('Flat glass'!$D$18+D11))*$H$2</f>
         <v>11.788444010275478</v>
       </c>
       <c r="F4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H4" s="5">
         <v>0.84530000000000005</v>
       </c>
       <c r="I4" s="5">
-        <f>H4+I20</f>
+        <f>H4+I15</f>
         <v>0.85530000000000006</v>
       </c>
       <c r="N4" s="4">
-        <f>(('Flat glass'!$D$19+N11))*$H$2</f>
+        <f>(('Flat glass'!$D$18+N11))*$H$2</f>
         <v>11.65061583290759</v>
       </c>
       <c r="O4" s="4">
-        <f>(('Flat glass'!$D$19+O11))*$H$2</f>
+        <f>(('Flat glass'!$D$18+O11))*$H$2</f>
         <v>11.788444010275478</v>
       </c>
       <c r="P4" s="4">
-        <f>(('Flat glass'!$D$19+P11))*$H$2</f>
+        <f>(('Flat glass'!$D$18+P11))*$H$2</f>
         <v>11.788444010275478</v>
       </c>
       <c r="Q4" s="4">
-        <f>(('Flat glass'!$D$19+Q11))*$H$2</f>
+        <f>(('Flat glass'!$D$18+Q11))*$H$2</f>
         <v>11.788444010275478</v>
       </c>
       <c r="S4" s="8">
@@ -1508,29 +1587,29 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" s="4">
         <f>(('Container glass'!$D$13+D9)-(SUM(D20:D22)))*$H$1</f>
         <v>13.58776385767761</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H5" s="5">
         <v>0.1</v>
       </c>
       <c r="I5" s="5">
-        <f>H5-I20</f>
+        <f>H5-I15</f>
         <v>9.0000000000000011E-2</v>
       </c>
       <c r="N5" s="4">
@@ -1568,29 +1647,29 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="4">
         <f>(('Container glass'!$D$13+D9)-(SUM(D20:D22)))*$H$3</f>
         <v>38.513822411409272</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H6" s="5">
         <v>0.15</v>
       </c>
       <c r="I6" s="5">
-        <f>H6-I20</f>
+        <f>H6-I15</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="N6" s="4">
@@ -1628,29 +1707,29 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D7" s="4">
         <f>(('Container glass'!$D$13+D9)-(SUM(D20:D22)))*$H$2</f>
         <v>8.5310056884214163</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H7" s="5">
         <v>0.75</v>
       </c>
       <c r="I7" s="5">
-        <f>H7+I20</f>
+        <f>H7+I15</f>
         <v>0.76</v>
       </c>
       <c r="N7" s="4">
@@ -1688,29 +1767,29 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D8" s="4">
         <f>SUM(D14:D16)/(1-$H$5)</f>
         <v>87.61150424219106</v>
       </c>
       <c r="F8" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H8" s="5">
         <v>0.2</v>
       </c>
       <c r="I8" s="7">
-        <f>H8-I20/2</f>
+        <f>H8-I15/2</f>
         <v>0.19500000000000001</v>
       </c>
       <c r="N8" s="4">
@@ -1748,29 +1827,29 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D9" s="4">
         <f>(('Container glass'!$D$13-SUM(D20:D22))/$H$4)*(1-$H$4)</f>
         <v>9.3798619758265307</v>
       </c>
       <c r="F9" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H9" s="5">
         <v>0.05</v>
       </c>
       <c r="I9" s="7">
-        <f>H9-I20/2</f>
+        <f>H9-I15/2</f>
         <v>4.5000000000000005E-2</v>
       </c>
       <c r="N9" s="4">
@@ -1808,45 +1887,45 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D10" s="4">
-        <f>'Flat glass'!$D$19/(1-$H$6)</f>
+        <f>'Flat glass'!$D$18/(1-$H$6)</f>
         <v>83.320972631680775</v>
       </c>
       <c r="F10" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="G10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H10" s="5">
         <v>0.83</v>
       </c>
       <c r="I10" s="5">
-        <f>H10+I20</f>
+        <f>H10+I15</f>
         <v>0.84</v>
       </c>
       <c r="N10" s="4">
-        <f>'Flat glass'!$D$19/(1-$H$6)</f>
+        <f>'Flat glass'!$D$18/(1-$H$6)</f>
         <v>83.320972631680775</v>
       </c>
       <c r="O10" s="4">
-        <f>'Flat glass'!$D$19/(1-$I$6)</f>
+        <f>'Flat glass'!$D$18/(1-$I$6)</f>
         <v>82.352124112707742</v>
       </c>
       <c r="P10" s="4">
-        <f>'Flat glass'!$D$19/(1-$H$6)</f>
+        <f>'Flat glass'!$D$18/(1-$H$6)</f>
         <v>83.320972631680775</v>
       </c>
       <c r="Q10" s="4">
-        <f>'Flat glass'!$D$19/(1-$H$6)</f>
+        <f>'Flat glass'!$D$18/(1-$H$6)</f>
         <v>83.320972631680775</v>
       </c>
       <c r="S10" s="8">
@@ -1868,45 +1947,45 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D11" s="4">
-        <f>('Flat glass'!$D$19/$H$4)*(1-$H$4)</f>
+        <f>('Flat glass'!$D$18/$H$4)*(1-$H$4)</f>
         <v>12.961423513785473</v>
       </c>
       <c r="F11" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H11" s="5">
         <v>0.06</v>
       </c>
       <c r="I11" s="7">
-        <f>H11-I20/2</f>
+        <f>H11-I15/2</f>
         <v>5.5E-2</v>
       </c>
       <c r="N11" s="4">
-        <f>('Flat glass'!$D$19/$I$4)*(1-$I$4)</f>
+        <f>('Flat glass'!$D$18/$I$4)*(1-$I$4)</f>
         <v>11.981834477766366</v>
       </c>
       <c r="O11" s="4">
-        <f>('Flat glass'!$D$19/$H$4)*(1-$H$4)</f>
+        <f>('Flat glass'!$D$18/$H$4)*(1-$H$4)</f>
         <v>12.961423513785473</v>
       </c>
       <c r="P11" s="4">
-        <f>('Flat glass'!$D$19/$H$4)*(1-$H$4)</f>
+        <f>('Flat glass'!$D$18/$H$4)*(1-$H$4)</f>
         <v>12.961423513785473</v>
       </c>
       <c r="Q11" s="4">
-        <f>('Flat glass'!$D$19/$H$4)*(1-$H$4)</f>
+        <f>('Flat glass'!$D$18/$H$4)*(1-$H$4)</f>
         <v>12.961423513785473</v>
       </c>
       <c r="S11" s="8">
@@ -1928,29 +2007,29 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
         <v>73</v>
-      </c>
-      <c r="C12" t="s">
-        <v>79</v>
       </c>
       <c r="D12" s="4">
         <f>(SUM(D14:D16)/(1-$H$5))-SUM(D14:D16)</f>
         <v>8.7611504242191103</v>
       </c>
       <c r="F12" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H12" s="5">
         <v>0.11</v>
       </c>
       <c r="I12" s="7">
-        <f>H12-I20/2</f>
+        <f>H12-I15/2</f>
         <v>0.105</v>
       </c>
       <c r="N12" s="4">
@@ -1988,45 +2067,45 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D13" s="4">
-        <f>('Flat glass'!$D$19/(1-$H$6))-'Flat glass'!$D$19</f>
+        <f>('Flat glass'!$D$18/(1-$H$6))-'Flat glass'!$D$18</f>
         <v>12.498145894752113</v>
       </c>
       <c r="F13" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="G13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H13" s="6">
         <v>0.35</v>
       </c>
       <c r="I13" s="6">
-        <f>H13+I20</f>
+        <f>H13+I15</f>
         <v>0.36</v>
       </c>
       <c r="N13" s="4">
-        <f>('Flat glass'!$D$19/(1-$H$6))-'Flat glass'!$D$19</f>
+        <f>('Flat glass'!$D$18/(1-$H$6))-'Flat glass'!$D$18</f>
         <v>12.498145894752113</v>
       </c>
       <c r="O13" s="4">
-        <f>('Flat glass'!$D$19/(1-$I$6))-'Flat glass'!$D$19</f>
+        <f>('Flat glass'!$D$18/(1-$I$6))-'Flat glass'!$D$18</f>
         <v>11.52929737577908</v>
       </c>
       <c r="P13" s="4">
-        <f>('Flat glass'!$D$19/(1-$H$6))-'Flat glass'!$D$19</f>
+        <f>('Flat glass'!$D$18/(1-$H$6))-'Flat glass'!$D$18</f>
         <v>12.498145894752113</v>
       </c>
       <c r="Q13" s="4">
-        <f>('Flat glass'!$D$19/(1-$H$6))-'Flat glass'!$D$19</f>
+        <f>('Flat glass'!$D$18/(1-$H$6))-'Flat glass'!$D$18</f>
         <v>12.498145894752113</v>
       </c>
       <c r="S13" s="8">
@@ -2048,13 +2127,13 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D14" s="4">
         <f>'Container glass'!$D$13*$H$7</f>
@@ -2096,18 +2175,24 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D15" s="4">
         <f>'Container glass'!$D$13*$H$8</f>
         <v>15.77007076359439</v>
       </c>
+      <c r="H15" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0.01</v>
+      </c>
       <c r="N15" s="4">
         <f>'Container glass'!$D$13*$H$8</f>
         <v>15.77007076359439</v>
@@ -2143,21 +2228,18 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D16" s="4">
         <f>'Container glass'!$D$13*$H$9</f>
         <v>3.9425176908985975</v>
       </c>
-      <c r="G16" t="s">
-        <v>48</v>
-      </c>
       <c r="N16" s="4">
         <f>'Container glass'!$D$13*$H$9</f>
         <v>3.9425176908985975</v>
@@ -2193,38 +2275,33 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D17" s="4">
-        <f>'Flat glass'!$D$19*$H$10</f>
+        <f>'Flat glass'!$D$18*$H$10</f>
         <v>58.782946191650787</v>
       </c>
-      <c r="G17" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0.37490000000000001</v>
-      </c>
+      <c r="H17" s="5"/>
       <c r="N17" s="4">
-        <f>'Flat glass'!$D$19*$H$10</f>
+        <f>'Flat glass'!$D$18*$H$10</f>
         <v>58.782946191650787</v>
       </c>
       <c r="O17" s="4">
-        <f>'Flat glass'!$D$19*$H$10</f>
+        <f>'Flat glass'!$D$18*$H$10</f>
         <v>58.782946191650787</v>
       </c>
       <c r="P17" s="4">
-        <f>'Flat glass'!$D$19*$I$10</f>
+        <f>'Flat glass'!$D$18*$I$10</f>
         <v>59.491174459020073</v>
       </c>
       <c r="Q17" s="4">
-        <f>'Flat glass'!$D$19*$H$10</f>
+        <f>'Flat glass'!$D$18*$H$10</f>
         <v>58.782946191650787</v>
       </c>
       <c r="S17" s="8">
@@ -2246,38 +2323,33 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D18" s="4">
-        <f>'Flat glass'!$D$19*$H$11</f>
+        <f>'Flat glass'!$D$18*$H$11</f>
         <v>4.2493696042157199</v>
       </c>
-      <c r="G18" t="s">
-        <v>52</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0.1298</v>
-      </c>
+      <c r="H18" s="5"/>
       <c r="N18" s="4">
-        <f>'Flat glass'!$D$19*$H$11</f>
+        <f>'Flat glass'!$D$18*$H$11</f>
         <v>4.2493696042157199</v>
       </c>
       <c r="O18" s="4">
-        <f>'Flat glass'!$D$19*$H$11</f>
+        <f>'Flat glass'!$D$18*$H$11</f>
         <v>4.2493696042157199</v>
       </c>
       <c r="P18" s="4">
-        <f>'Flat glass'!$D$19*$I$11</f>
+        <f>'Flat glass'!$D$18*$I$11</f>
         <v>3.8952554705310765</v>
       </c>
       <c r="Q18" s="4">
-        <f>'Flat glass'!$D$19*$H$11</f>
+        <f>'Flat glass'!$D$18*$H$11</f>
         <v>4.2493696042157199</v>
       </c>
       <c r="S18" s="8">
@@ -2299,32 +2371,32 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D19" s="4">
-        <f>'Flat glass'!$D$19*$H$12</f>
+        <f>'Flat glass'!$D$18*$H$12</f>
         <v>7.7905109410621529</v>
       </c>
       <c r="N19" s="4">
-        <f>'Flat glass'!$D$19*$H$12</f>
+        <f>'Flat glass'!$D$18*$H$12</f>
         <v>7.7905109410621529</v>
       </c>
       <c r="O19" s="4">
-        <f>'Flat glass'!$D$19*$H$12</f>
+        <f>'Flat glass'!$D$18*$H$12</f>
         <v>7.7905109410621529</v>
       </c>
       <c r="P19" s="4">
-        <f>'Flat glass'!$D$19*$I$12</f>
+        <f>'Flat glass'!$D$18*$I$12</f>
         <v>7.4363968073775091</v>
       </c>
       <c r="Q19" s="4">
-        <f>'Flat glass'!$D$19*$H$12</f>
+        <f>'Flat glass'!$D$18*$H$12</f>
         <v>7.7905109410621529</v>
       </c>
       <c r="S19" s="8">
@@ -2346,34 +2418,28 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D20" s="4">
         <f>D14*$H$13</f>
         <v>20.698217877217637</v>
       </c>
-      <c r="H20" t="s">
-        <v>85</v>
-      </c>
-      <c r="I20" s="6">
-        <v>0.01</v>
-      </c>
       <c r="N20" s="4">
-        <f>N14*$H$13</f>
+        <f t="shared" ref="N20:P22" si="4">N14*$H$13</f>
         <v>20.698217877217637</v>
       </c>
       <c r="O20" s="4">
-        <f>O14*$H$13</f>
+        <f t="shared" si="4"/>
         <v>20.698217877217637</v>
       </c>
       <c r="P20" s="4">
-        <f>P14*$H$13</f>
+        <f t="shared" si="4"/>
         <v>20.974194115580538</v>
       </c>
       <c r="Q20" s="4">
@@ -2399,28 +2465,28 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D21" s="4">
         <f>D15*$H$13</f>
         <v>5.5195247672580363</v>
       </c>
       <c r="N21" s="4">
-        <f>N15*$H$13</f>
+        <f t="shared" si="4"/>
         <v>5.5195247672580363</v>
       </c>
       <c r="O21" s="4">
-        <f>O15*$H$13</f>
+        <f t="shared" si="4"/>
         <v>5.5195247672580363</v>
       </c>
       <c r="P21" s="4">
-        <f>P15*$H$13</f>
+        <f t="shared" si="4"/>
         <v>5.3815366480765858</v>
       </c>
       <c r="Q21" s="4">
@@ -2446,28 +2512,28 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D22" s="4">
         <f>D16*$H$13</f>
         <v>1.3798811918145091</v>
       </c>
       <c r="N22" s="4">
-        <f>N16*$H$13</f>
+        <f t="shared" si="4"/>
         <v>1.3798811918145091</v>
       </c>
       <c r="O22" s="4">
-        <f>O16*$H$13</f>
+        <f t="shared" si="4"/>
         <v>1.3798811918145091</v>
       </c>
       <c r="P22" s="4">
-        <f>P16*$H$13</f>
+        <f t="shared" si="4"/>
         <v>1.2418930726330581</v>
       </c>
       <c r="Q22" s="4">
@@ -2493,28 +2559,28 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D23" s="4">
         <f>D14*(1-$H$13)</f>
         <v>38.439547486261326</v>
       </c>
       <c r="N23" s="4">
-        <f>N14*(1-$H$13)</f>
+        <f t="shared" ref="N23:P25" si="5">N14*(1-$H$13)</f>
         <v>38.439547486261326</v>
       </c>
       <c r="O23" s="4">
-        <f>O14*(1-$H$13)</f>
+        <f t="shared" si="5"/>
         <v>38.439547486261326</v>
       </c>
       <c r="P23" s="4">
-        <f>P14*(1-$H$13)</f>
+        <f t="shared" si="5"/>
         <v>38.952074786078143</v>
       </c>
       <c r="Q23" s="4">
@@ -2540,28 +2606,28 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D24" s="4">
         <f>D15*(1-$H$13)</f>
         <v>10.250545996336355</v>
       </c>
       <c r="N24" s="4">
-        <f>N15*(1-$H$13)</f>
+        <f t="shared" si="5"/>
         <v>10.250545996336355</v>
       </c>
       <c r="O24" s="4">
-        <f>O15*(1-$H$13)</f>
+        <f t="shared" si="5"/>
         <v>10.250545996336355</v>
       </c>
       <c r="P24" s="4">
-        <f>P15*(1-$H$13)</f>
+        <f t="shared" si="5"/>
         <v>9.994282346427946</v>
       </c>
       <c r="Q24" s="4">
@@ -2587,28 +2653,28 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D25" s="4">
         <f>D16*(1-$H$13)</f>
         <v>2.5626364990840886</v>
       </c>
       <c r="N25" s="4">
-        <f>N16*(1-$H$13)</f>
+        <f t="shared" si="5"/>
         <v>2.5626364990840886</v>
       </c>
       <c r="O25" s="4">
-        <f>O16*(1-$H$13)</f>
+        <f t="shared" si="5"/>
         <v>2.5626364990840886</v>
       </c>
       <c r="P25" s="4">
-        <f>P16*(1-$H$13)</f>
+        <f t="shared" si="5"/>
         <v>2.3063728491756796</v>
       </c>
       <c r="Q25" s="4">
@@ -2634,20 +2700,17 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D26" s="4">
-        <f>4.3+2.7+12.5+0.4+0.4+0.1</f>
-        <v>20.399999999999999</v>
-      </c>
-      <c r="E26" t="s">
-        <v>57</v>
+        <f>'Flat glass'!D20</f>
+        <v>12.4</v>
       </c>
       <c r="N26" s="4">
         <f>4.3+2.7+12.5+0.4+0.4+0.1</f>
@@ -2667,37 +2730,34 @@
       </c>
       <c r="S26" s="8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.6451612903225805</v>
       </c>
       <c r="T26" s="8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.6451612903225805</v>
       </c>
       <c r="U26" s="8">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.6451612903225805</v>
       </c>
       <c r="V26" s="8">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>1.6451612903225805</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D27" s="4">
-        <f>(0.15+0.25+0.08+0.1)*100/(15+16+16+28)</f>
+        <f>'Flat glass'!D21</f>
         <v>0.77333333333333343</v>
-      </c>
-      <c r="E27" t="s">
-        <v>58</v>
       </c>
       <c r="N27" s="4">
         <f>(0.15+0.25+0.08+0.1)*100/(15+16+16+28)</f>
@@ -2734,28 +2794,28 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="X30" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="Y30" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="Z30" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="AA30" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="AB30" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="AC30" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AD30" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="AE30" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
@@ -2768,7 +2828,7 @@
         <v>loss1</v>
       </c>
       <c r="Z31" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="AA31" t="s">
         <v>5</v>
@@ -2778,10 +2838,10 @@
         <v>0.92442272756713495</v>
       </c>
       <c r="AC31" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AD31" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AE31" s="9">
         <f>V9</f>
@@ -2790,15 +2850,15 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="X32" t="str">
-        <f>A11</f>
+        <f t="shared" ref="X32:Y34" si="6">A11</f>
         <v>FGM</v>
       </c>
       <c r="Y32" t="str">
-        <f>B11</f>
+        <f t="shared" si="6"/>
         <v>loss2</v>
       </c>
       <c r="Z32" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="AA32" t="s">
         <v>5</v>
@@ -2808,71 +2868,71 @@
         <v>0.92442272756713506</v>
       </c>
       <c r="AC32" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AD32" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AE32" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X33" t="str">
-        <f>A12</f>
+        <f t="shared" si="6"/>
         <v>CGF</v>
       </c>
       <c r="Y33" t="str">
-        <f>B12</f>
+        <f t="shared" si="6"/>
         <v>CGM</v>
       </c>
       <c r="Z33" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="AA33" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="AB33" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AC33" s="9">
         <f>T12</f>
         <v>0.89010989010988961</v>
       </c>
       <c r="AD33" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AE33" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X34" t="str">
-        <f>A13</f>
+        <f t="shared" si="6"/>
         <v>FGF</v>
       </c>
       <c r="Y34" t="str">
-        <f>B13</f>
+        <f t="shared" si="6"/>
         <v>FGM</v>
       </c>
       <c r="Z34" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="AA34" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="AB34" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AC34" s="9">
         <f>T13</f>
         <v>0.92248062015503873</v>
       </c>
       <c r="AD34" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AE34" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="24:31" x14ac:dyDescent="0.25">
@@ -2885,103 +2945,103 @@
         <v>CGU</v>
       </c>
       <c r="Z35" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="AA35" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="AB35" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AC35" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AD35" s="9">
         <f>U16</f>
         <v>0.9</v>
       </c>
       <c r="AE35" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X36" t="str">
-        <f>A18</f>
+        <f t="shared" ref="X36:Y40" si="7">A18</f>
         <v>FGF</v>
       </c>
       <c r="Y36" t="str">
-        <f>B18</f>
+        <f t="shared" si="7"/>
         <v>FGU</v>
       </c>
       <c r="Z36" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="AA36" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="AB36" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AC36" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AD36" s="9">
         <f>U18</f>
         <v>0.91666666666666663</v>
       </c>
       <c r="AE36" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X37" t="str">
-        <f>A19</f>
+        <f t="shared" si="7"/>
         <v>FGF</v>
       </c>
       <c r="Y37" t="str">
-        <f>B19</f>
+        <f t="shared" si="7"/>
         <v>FGU</v>
       </c>
       <c r="Z37" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="AA37" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="AB37" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AC37" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AD37" s="9">
         <f>U19</f>
         <v>0.95454545454545447</v>
       </c>
       <c r="AE37" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X38" t="str">
-        <f>A20</f>
+        <f t="shared" si="7"/>
         <v>CGU</v>
       </c>
       <c r="Y38" t="str">
-        <f>B20</f>
+        <f t="shared" si="7"/>
         <v>CGM</v>
       </c>
       <c r="Z38" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="AA38" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="AB38" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AC38" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AD38" s="9">
         <f>U20</f>
@@ -2994,24 +3054,24 @@
     </row>
     <row r="39" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X39" t="str">
-        <f>A21</f>
+        <f t="shared" si="7"/>
         <v>CGU</v>
       </c>
       <c r="Y39" t="str">
-        <f>B21</f>
+        <f t="shared" si="7"/>
         <v>CGM</v>
       </c>
       <c r="Z39" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="AA39" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="AB39" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AC39" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AD39" s="9">
         <f>U21</f>
@@ -3024,24 +3084,24 @@
     </row>
     <row r="40" spans="24:31" x14ac:dyDescent="0.25">
       <c r="X40" t="str">
-        <f>A22</f>
+        <f t="shared" si="7"/>
         <v>CGU</v>
       </c>
       <c r="Y40" t="str">
-        <f>B22</f>
+        <f t="shared" si="7"/>
         <v>CGM</v>
       </c>
       <c r="Z40" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="AA40" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="AB40" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AC40" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AD40" s="9">
         <f>U22</f>
@@ -3062,16 +3122,16 @@
         <v>EoL</v>
       </c>
       <c r="Z41" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="AA41" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="AB41" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AC41" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AD41" s="9">
         <f>U25</f>
@@ -3097,4 +3157,108 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C5F011-9BE9-4369-9A3B-10B4B1EB8745}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2006</v>
+      </c>
+      <c r="B2" s="2">
+        <f>'Flat glass'!D19</f>
+        <v>2.69</v>
+      </c>
+      <c r="C2" s="2">
+        <f>'Flat glass'!D5*Flows!H10</f>
+        <v>36.519999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2014</v>
+      </c>
+      <c r="B3" s="2">
+        <f>Flows!D26</f>
+        <v>12.4</v>
+      </c>
+      <c r="C3" s="2">
+        <f>Flows!D17</f>
+        <v>58.782946191650787</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFBE00B-16BB-4492-A6C9-F4C0D6C72784}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2006</v>
+      </c>
+      <c r="B2" s="2">
+        <f>'Flat glass'!D22</f>
+        <v>0.23</v>
+      </c>
+      <c r="C2" s="2">
+        <f>'Flat glass'!D5*Flows!H11</f>
+        <v>2.6399999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2014</v>
+      </c>
+      <c r="B3" s="2">
+        <f>'Flat glass'!D21</f>
+        <v>0.77333333333333343</v>
+      </c>
+      <c r="C3" s="2">
+        <f>Flows!D18</f>
+        <v>4.2493696042157199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added some numbers to glass_paper.xlsx and edited the dynamic stock model graphs
</commit_message>
<xml_diff>
--- a/data/glass_paper.xlsx
+++ b/data/glass_paper.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Desktop\python\glass-paper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350917CF-10AA-463C-B610-EB2A7DE5ED26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80CD64D-A4B3-443E-8868-43E84FA63DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{1AC0E601-1297-4C8D-8E5F-6A8C787FDED8}"/>
+    <workbookView xWindow="20370" yWindow="-5925" windowWidth="30960" windowHeight="16920" activeTab="5" xr2:uid="{1AC0E601-1297-4C8D-8E5F-6A8C787FDED8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mentioned_numbers" sheetId="1" r:id="rId1"/>
     <sheet name="Container glass" sheetId="4" r:id="rId2"/>
     <sheet name="Flat glass" sheetId="2" r:id="rId3"/>
     <sheet name="Flows" sheetId="3" r:id="rId4"/>
@@ -38,35 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="110">
-  <si>
-    <t>Global production of glass</t>
-  </si>
-  <si>
-    <t>Global emissions of glass</t>
-  </si>
-  <si>
-    <t>Figures to synchronise (hopefully for 2014)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Global energy of glass production </t>
-  </si>
-  <si>
-    <t>Mentioned twice in introduction</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="119">
   <si>
     <t>Process emissions</t>
   </si>
   <si>
-    <t>Combustion emissions</t>
-  </si>
-  <si>
-    <t>Indirect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total </t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -368,6 +344,57 @@
   </si>
   <si>
     <t>Table 11.7: https://www.sciencedirect.com/science/article/pii/B9780123814753100117</t>
+  </si>
+  <si>
+    <t>Energy intensity</t>
+  </si>
+  <si>
+    <t>CO2 intensity</t>
+  </si>
+  <si>
+    <t>For the "EU25 glass industry", taken from https://www.sciencedirect.com/science/article/pii/S0301421510007081</t>
+  </si>
+  <si>
+    <t>kg CO2 / kg</t>
+  </si>
+  <si>
+    <t>GJ/t</t>
+  </si>
+  <si>
+    <t>https://www.iea.org/articles/global-co2-emissions-in-2019</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Glass global emissions percentage</t>
+  </si>
+  <si>
+    <t>Global emissions in 2014 [Gt]</t>
+  </si>
+  <si>
+    <t>Mt</t>
+  </si>
+  <si>
+    <t>Butler &amp; Hooper (2011)</t>
+  </si>
+  <si>
+    <t>(European Commission, 2008)</t>
+  </si>
+  <si>
+    <t>(British Glass, 2008)</t>
+  </si>
+  <si>
+    <t>Estimated in supporting information</t>
+  </si>
+  <si>
+    <t>Table 3 of manuscript from here</t>
+  </si>
+  <si>
+    <t>Global glass production in 2014</t>
+  </si>
+  <si>
+    <t>Global glass emissions in 2014</t>
   </si>
 </sst>
 </file>
@@ -378,7 +405,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,6 +436,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -432,7 +467,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -446,6 +481,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -762,83 +798,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D74802-20F5-460E-AF3A-FC01A078C0A6}">
-  <dimension ref="B2:D14"/>
+  <dimension ref="B2:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>2</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>0</v>
+        <v>102</v>
+      </c>
+      <c r="C3">
+        <v>7.8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>4.45</v>
-      </c>
-      <c r="D10">
-        <f>C10/$C$14</f>
-        <v>0.16457100591715978</v>
+        <v>103</v>
+      </c>
+      <c r="C4">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6">
+        <f>'Container glass'!D3+'Flat glass'!D4</f>
+        <v>150.19999999999999</v>
+      </c>
+      <c r="D6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="4">
+        <f>C6*C4</f>
+        <v>85.61399999999999</v>
+      </c>
+      <c r="D7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9">
+        <f>20.5+11.8</f>
+        <v>32.299999999999997</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11">
-        <v>16.89</v>
-      </c>
-      <c r="D11">
-        <f t="shared" ref="D11:D12" si="0">C11/$C$14</f>
-        <v>0.62463017751479299</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12">
-        <v>5.7</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0.21079881656804736</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14">
-        <f>SUM(C10:C12)</f>
-        <v>27.04</v>
+        <v>109</v>
+      </c>
+      <c r="C11" s="2">
+        <f>C7/(C9*1000)*100</f>
+        <v>0.26505882352941179</v>
+      </c>
+      <c r="D11" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{67A8E8E8-FF10-43BB-AFAA-918C967621FB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -848,7 +897,7 @@
   <dimension ref="B2:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B13" sqref="B13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,21 +907,21 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C3">
         <v>2014</v>
@@ -881,12 +930,12 @@
         <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <v>2007</v>
@@ -895,12 +944,12 @@
         <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C5">
         <v>2007</v>
@@ -910,12 +959,12 @@
         <v>39851</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>2014</v>
@@ -925,12 +974,12 @@
         <v>44959</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C7">
         <v>2014</v>
@@ -940,12 +989,12 @@
         <v>80.700707635943886</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C8">
         <v>2007</v>
@@ -954,12 +1003,12 @@
         <v>4.2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C9">
         <v>2014</v>
@@ -968,12 +1017,12 @@
         <v>4</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C10">
         <v>2007</v>
@@ -982,12 +1031,12 @@
         <v>0.7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C11">
         <v>2014</v>
@@ -996,22 +1045,22 @@
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="10">
         <v>2014</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="11">
         <f>AVERAGE(D7,D3)</f>
         <v>78.85035381797195</v>
       </c>
-      <c r="E13" t="s">
-        <v>28</v>
+      <c r="E13" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1029,35 +1078,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EC93BF-3E27-439B-9576-A211E3A0EC5A}">
-  <dimension ref="B2:F22"/>
+  <dimension ref="B2:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>17</v>
       </c>
       <c r="C3">
         <v>2014</v>
@@ -1066,15 +1115,15 @@
         <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>2015</v>
@@ -1083,12 +1132,12 @@
         <v>73.2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>2006</v>
@@ -1097,12 +1146,12 @@
         <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>2014</v>
@@ -1111,12 +1160,12 @@
         <v>41.56</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>2014</v>
@@ -1125,12 +1174,12 @@
         <v>9.2799999999999994</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>2014</v>
@@ -1139,12 +1188,12 @@
         <v>3.53</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>2006</v>
@@ -1153,12 +1202,12 @@
         <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>2006</v>
@@ -1167,12 +1216,12 @@
         <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>2006</v>
@@ -1181,12 +1230,12 @@
         <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>2014</v>
@@ -1196,12 +1245,13 @@
         <v>75.513888888888886</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <v>2010</v>
@@ -1210,12 +1260,12 @@
         <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>2018</v>
@@ -1224,12 +1274,12 @@
         <v>10.6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>2010</v>
@@ -1239,12 +1289,12 @@
         <v>87208</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>2014</v>
@@ -1254,12 +1304,12 @@
         <v>116204</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C17" s="4">
         <v>2014</v>
@@ -1269,12 +1319,12 @@
         <v>71.95459132189707</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C18" s="10">
         <v>2014</v>
@@ -1284,12 +1334,12 @@
         <v>70.822826736928661</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C19">
         <v>2006</v>
@@ -1299,12 +1349,12 @@
         <v>2.69</v>
       </c>
       <c r="E19" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C20">
         <v>2014</v>
@@ -1314,12 +1364,12 @@
         <v>12.4</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C21">
         <v>2014</v>
@@ -1329,12 +1379,12 @@
         <v>0.77333333333333343</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C22">
         <v>2006</v>
@@ -1344,8 +1394,11 @@
         <v>0.23</v>
       </c>
       <c r="E22" t="s">
-        <v>109</v>
-      </c>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1362,10 +1415,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11B3549B-C2AB-4D75-AB88-A04A3C1A4639}">
-  <dimension ref="A1:AE41"/>
+  <dimension ref="A1:AE27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,69 +1428,78 @@
     <col min="7" max="7" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H1" s="5">
         <v>0.22409999999999999</v>
       </c>
+      <c r="I1" t="s">
+        <v>115</v>
+      </c>
       <c r="N1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="O1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="P1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="Q1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="S1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="T1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="U1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="V1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="X1" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D2" s="4">
         <f>(('Flat glass'!$D$18+D11))*$H$1</f>
         <v>18.776050481185038</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H2" s="5">
         <v>0.14069999999999999</v>
+      </c>
+      <c r="I2" t="s">
+        <v>115</v>
       </c>
       <c r="N2" s="4">
         <f>(('Flat glass'!$D$18+N11))*$H$1</f>
@@ -1471,26 +1533,53 @@
         <f>Q2/$D2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D3" s="4">
         <f>(('Flat glass'!$D$18+D11))*$H$3</f>
         <v>53.219755759253616</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="H3" s="5">
         <v>0.63519999999999999</v>
+      </c>
+      <c r="I3" t="s">
+        <v>115</v>
       </c>
       <c r="N3" s="4">
         <f>(('Flat glass'!$D$18+N11))*$H$3</f>
@@ -1524,32 +1613,63 @@
         <f t="shared" ref="V3:V27" si="3">Q3/$D3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X3" t="str">
+        <f>A9</f>
+        <v>CGM</v>
+      </c>
+      <c r="Y3" t="str">
+        <f>B9</f>
+        <v>loss1</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="9">
+        <f>S9</f>
+        <v>0.92442272756713495</v>
+      </c>
+      <c r="AC3" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD3" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE3" s="9">
+        <f>V9</f>
+        <v>0.98461538461538456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D4" s="4">
         <f>(('Flat glass'!$D$18+D11))*$H$2</f>
         <v>11.788444010275478</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H4" s="5">
         <v>0.84530000000000005</v>
       </c>
-      <c r="I4" s="5">
-        <f>H4+I15</f>
+      <c r="I4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K4" s="5">
+        <f>H4+K15</f>
         <v>0.85530000000000006</v>
       </c>
       <c r="N4" s="4">
@@ -1584,32 +1704,62 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X4" t="str">
+        <f>A11</f>
+        <v>FGM</v>
+      </c>
+      <c r="Y4" t="str">
+        <f>B11</f>
+        <v>loss2</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="9">
+        <f>S11</f>
+        <v>0.92442272756713506</v>
+      </c>
+      <c r="AC4" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD4" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE4" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D5" s="4">
         <f>(('Container glass'!$D$13+D9)-(SUM(D20:D22)))*$H$1</f>
         <v>13.58776385767761</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H5" s="5">
         <v>0.1</v>
       </c>
-      <c r="I5" s="5">
-        <f>H5-I15</f>
+      <c r="I5" t="s">
+        <v>114</v>
+      </c>
+      <c r="K5" s="5">
+        <f>H5-K15</f>
         <v>9.0000000000000011E-2</v>
       </c>
       <c r="N5" s="4">
@@ -1644,32 +1794,62 @@
         <f t="shared" si="3"/>
         <v>0.98461538461538467</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X5" t="str">
+        <f>A12</f>
+        <v>CGF</v>
+      </c>
+      <c r="Y5" t="str">
+        <f>B12</f>
+        <v>CGM</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB5" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC5" s="9">
+        <f>T12</f>
+        <v>0.89010989010988961</v>
+      </c>
+      <c r="AD5" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE5" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D6" s="4">
         <f>(('Container glass'!$D$13+D9)-(SUM(D20:D22)))*$H$3</f>
         <v>38.513822411409272</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H6" s="5">
         <v>0.15</v>
       </c>
-      <c r="I6" s="5">
-        <f>H6-I15</f>
+      <c r="I6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K6" s="5">
+        <f>H6-K15</f>
         <v>0.13999999999999999</v>
       </c>
       <c r="N6" s="4">
@@ -1704,32 +1884,62 @@
         <f t="shared" si="3"/>
         <v>0.98461538461538456</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X6" t="str">
+        <f>A13</f>
+        <v>FGF</v>
+      </c>
+      <c r="Y6" t="str">
+        <f>B13</f>
+        <v>FGM</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB6" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC6" s="9">
+        <f>T13</f>
+        <v>0.92248062015503873</v>
+      </c>
+      <c r="AD6" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE6" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D7" s="4">
         <f>(('Container glass'!$D$13+D9)-(SUM(D20:D22)))*$H$2</f>
         <v>8.5310056884214163</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H7" s="5">
         <v>0.75</v>
       </c>
-      <c r="I7" s="5">
-        <f>H7+I15</f>
+      <c r="I7" t="s">
+        <v>113</v>
+      </c>
+      <c r="K7" s="5">
+        <f>H7+K15</f>
         <v>0.76</v>
       </c>
       <c r="N7" s="4">
@@ -1764,32 +1974,62 @@
         <f t="shared" si="3"/>
         <v>0.98461538461538478</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X7" t="str">
+        <f>A16</f>
+        <v>CGF</v>
+      </c>
+      <c r="Y7" t="str">
+        <f>B16</f>
+        <v>CGU</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB7" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC7" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD7" s="9">
+        <f>U16</f>
+        <v>0.9</v>
+      </c>
+      <c r="AE7" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D8" s="4">
         <f>SUM(D14:D16)/(1-$H$5)</f>
         <v>87.61150424219106</v>
       </c>
       <c r="F8" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="H8" s="5">
         <v>0.2</v>
       </c>
-      <c r="I8" s="7">
-        <f>H8-I15/2</f>
+      <c r="I8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K8" s="7">
+        <f>H8-K15/2</f>
         <v>0.19500000000000001</v>
       </c>
       <c r="N8" s="4">
@@ -1797,7 +2037,7 @@
         <v>87.61150424219106</v>
       </c>
       <c r="O8" s="4">
-        <f>SUM(O14:O16)/(1-$I$5)</f>
+        <f>SUM(O14:O16)/(1-$K$5)</f>
         <v>86.648740459309835</v>
       </c>
       <c r="P8" s="4">
@@ -1824,36 +2064,66 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X8" t="str">
+        <f>A18</f>
+        <v>FGF</v>
+      </c>
+      <c r="Y8" t="str">
+        <f>B18</f>
+        <v>FGU</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB8" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC8" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD8" s="9">
+        <f>U18</f>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="AE8" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D9" s="4">
         <f>(('Container glass'!$D$13-SUM(D20:D22))/$H$4)*(1-$H$4)</f>
         <v>9.3798619758265307</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="H9" s="5">
         <v>0.05</v>
       </c>
-      <c r="I9" s="7">
-        <f>H9-I15/2</f>
+      <c r="I9" t="s">
+        <v>113</v>
+      </c>
+      <c r="K9" s="7">
+        <f>H9-K15/2</f>
         <v>4.5000000000000005E-2</v>
       </c>
       <c r="N9" s="4">
-        <f>(('Container glass'!$D$13-SUM(N20:N22))/$I$4)*(1-$I$4)</f>
+        <f>(('Container glass'!$D$13-SUM(N20:N22))/$K$4)*(1-$K$4)</f>
         <v>8.6709575918968174</v>
       </c>
       <c r="O9" s="4">
@@ -1884,32 +2154,62 @@
         <f t="shared" si="3"/>
         <v>0.98461538461538456</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X9" t="str">
+        <f>A19</f>
+        <v>FGF</v>
+      </c>
+      <c r="Y9" t="str">
+        <f>B19</f>
+        <v>FGU</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB9" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC9" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD9" s="9">
+        <f>U19</f>
+        <v>0.95454545454545447</v>
+      </c>
+      <c r="AE9" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D10" s="4">
         <f>'Flat glass'!$D$18/(1-$H$6)</f>
         <v>83.320972631680775</v>
       </c>
       <c r="F10" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H10" s="5">
         <v>0.83</v>
       </c>
-      <c r="I10" s="5">
-        <f>H10+I15</f>
+      <c r="I10" t="s">
+        <v>95</v>
+      </c>
+      <c r="K10" s="5">
+        <f>H10+K15</f>
         <v>0.84</v>
       </c>
       <c r="N10" s="4">
@@ -1917,7 +2217,7 @@
         <v>83.320972631680775</v>
       </c>
       <c r="O10" s="4">
-        <f>'Flat glass'!$D$18/(1-$I$6)</f>
+        <f>'Flat glass'!$D$18/(1-$K$6)</f>
         <v>82.352124112707742</v>
       </c>
       <c r="P10" s="4">
@@ -1944,36 +2244,67 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X10" t="str">
+        <f>A20</f>
+        <v>CGU</v>
+      </c>
+      <c r="Y10" t="str">
+        <f>B20</f>
+        <v>CGM</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB10" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC10" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD10" s="9">
+        <f>U20</f>
+        <v>1.0133333333333332</v>
+      </c>
+      <c r="AE10" s="9">
+        <f>V20</f>
+        <v>1.0285714285714287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D11" s="4">
         <f>('Flat glass'!$D$18/$H$4)*(1-$H$4)</f>
         <v>12.961423513785473</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G11" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H11" s="5">
         <v>0.06</v>
       </c>
-      <c r="I11" s="7">
-        <f>H11-I15/2</f>
+      <c r="I11" t="s">
+        <v>95</v>
+      </c>
+      <c r="K11" s="7">
+        <f>H11-K15/2</f>
         <v>5.5E-2</v>
       </c>
       <c r="N11" s="4">
-        <f>('Flat glass'!$D$18/$I$4)*(1-$I$4)</f>
+        <f>('Flat glass'!$D$18/$K$4)*(1-$K$4)</f>
         <v>11.981834477766366</v>
       </c>
       <c r="O11" s="4">
@@ -2004,32 +2335,63 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X11" t="str">
+        <f>A21</f>
+        <v>CGU</v>
+      </c>
+      <c r="Y11" t="str">
+        <f>B21</f>
+        <v>CGM</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB11" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC11" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD11" s="9">
+        <f>U21</f>
+        <v>0.97500000000000009</v>
+      </c>
+      <c r="AE11" s="9">
+        <f>V21</f>
+        <v>1.0285714285714285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D12" s="4">
         <f>(SUM(D14:D16)/(1-$H$5))-SUM(D14:D16)</f>
         <v>8.7611504242191103</v>
       </c>
       <c r="F12" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H12" s="5">
         <v>0.11</v>
       </c>
-      <c r="I12" s="7">
-        <f>H12-I15/2</f>
+      <c r="I12" t="s">
+        <v>95</v>
+      </c>
+      <c r="K12" s="7">
+        <f>H12-K15/2</f>
         <v>0.105</v>
       </c>
       <c r="N12" s="4">
@@ -2037,7 +2399,7 @@
         <v>8.7611504242191103</v>
       </c>
       <c r="O12" s="4">
-        <f>(SUM(O14:O16)/(1-$I$5))-SUM(O14:O16)</f>
+        <f>(SUM(O14:O16)/(1-$K$5))-SUM(O14:O16)</f>
         <v>7.7983866413378848</v>
       </c>
       <c r="P12" s="4">
@@ -2064,32 +2426,63 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X12" t="str">
+        <f>A22</f>
+        <v>CGU</v>
+      </c>
+      <c r="Y12" t="str">
+        <f>B22</f>
+        <v>CGM</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB12" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC12" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD12" s="9">
+        <f>U22</f>
+        <v>0.9</v>
+      </c>
+      <c r="AE12" s="9">
+        <f>V22</f>
+        <v>1.0285714285714285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D13" s="4">
         <f>('Flat glass'!$D$18/(1-$H$6))-'Flat glass'!$D$18</f>
         <v>12.498145894752113</v>
       </c>
       <c r="F13" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H13" s="6">
         <v>0.35</v>
       </c>
-      <c r="I13" s="6">
-        <f>H13+I15</f>
+      <c r="I13" t="s">
+        <v>112</v>
+      </c>
+      <c r="K13" s="6">
+        <f>H13+K15</f>
         <v>0.36</v>
       </c>
       <c r="N13" s="4">
@@ -2097,7 +2490,7 @@
         <v>12.498145894752113</v>
       </c>
       <c r="O13" s="4">
-        <f>('Flat glass'!$D$18/(1-$I$6))-'Flat glass'!$D$18</f>
+        <f>('Flat glass'!$D$18/(1-$K$6))-'Flat glass'!$D$18</f>
         <v>11.52929737577908</v>
       </c>
       <c r="P13" s="4">
@@ -2124,16 +2517,44 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X13" t="str">
+        <f>A25</f>
+        <v>CGU</v>
+      </c>
+      <c r="Y13" t="str">
+        <f>B25</f>
+        <v>EoL</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB13" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC13" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD13" s="9">
+        <f>U25</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="AE13" s="9">
+        <f>V25</f>
+        <v>0.98461538461538456</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D14" s="4">
         <f>'Container glass'!$D$13*$H$7</f>
@@ -2149,7 +2570,7 @@
         <v>59.137765363478962</v>
       </c>
       <c r="P14" s="4">
-        <f>'Container glass'!$D$13*$I$7</f>
+        <f>'Container glass'!$D$13*$K$7</f>
         <v>59.92626890165868</v>
       </c>
       <c r="Q14" s="4">
@@ -2173,24 +2594,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D15" s="4">
         <f>'Container glass'!$D$13*$H$8</f>
         <v>15.77007076359439</v>
       </c>
-      <c r="H15" t="s">
-        <v>102</v>
-      </c>
-      <c r="I15" s="6">
+      <c r="J15" t="s">
+        <v>94</v>
+      </c>
+      <c r="K15" s="6">
         <v>0.01</v>
       </c>
       <c r="N15" s="4">
@@ -2202,7 +2623,7 @@
         <v>15.77007076359439</v>
       </c>
       <c r="P15" s="4">
-        <f>'Container glass'!$D$13*$I$8</f>
+        <f>'Container glass'!$D$13*$K$8</f>
         <v>15.375818994504531</v>
       </c>
       <c r="Q15" s="4">
@@ -2226,15 +2647,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D16" s="4">
         <f>'Container glass'!$D$13*$H$9</f>
@@ -2249,7 +2670,7 @@
         <v>3.9425176908985975</v>
       </c>
       <c r="P16" s="4">
-        <f>'Container glass'!$D$13*$I$9</f>
+        <f>'Container glass'!$D$13*$K$9</f>
         <v>3.548265921808738</v>
       </c>
       <c r="Q16" s="4">
@@ -2273,15 +2694,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D17" s="4">
         <f>'Flat glass'!$D$18*$H$10</f>
@@ -2297,7 +2718,7 @@
         <v>58.782946191650787</v>
       </c>
       <c r="P17" s="4">
-        <f>'Flat glass'!$D$18*$I$10</f>
+        <f>'Flat glass'!$D$18*$K$10</f>
         <v>59.491174459020073</v>
       </c>
       <c r="Q17" s="4">
@@ -2321,15 +2742,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D18" s="4">
         <f>'Flat glass'!$D$18*$H$11</f>
@@ -2345,7 +2766,7 @@
         <v>4.2493696042157199</v>
       </c>
       <c r="P18" s="4">
-        <f>'Flat glass'!$D$18*$I$11</f>
+        <f>'Flat glass'!$D$18*$K$11</f>
         <v>3.8952554705310765</v>
       </c>
       <c r="Q18" s="4">
@@ -2369,15 +2790,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D19" s="4">
         <f>'Flat glass'!$D$18*$H$12</f>
@@ -2392,7 +2813,7 @@
         <v>7.7905109410621529</v>
       </c>
       <c r="P19" s="4">
-        <f>'Flat glass'!$D$18*$I$12</f>
+        <f>'Flat glass'!$D$18*$K$12</f>
         <v>7.4363968073775091</v>
       </c>
       <c r="Q19" s="4">
@@ -2416,15 +2837,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D20" s="4">
         <f>D14*$H$13</f>
@@ -2443,7 +2864,7 @@
         <v>20.974194115580538</v>
       </c>
       <c r="Q20" s="4">
-        <f>Q14*$I$13</f>
+        <f>Q14*$K$13</f>
         <v>21.289595530852427</v>
       </c>
       <c r="S20" s="8">
@@ -2463,15 +2884,15 @@
         <v>1.0285714285714287</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D21" s="4">
         <f>D15*$H$13</f>
@@ -2490,7 +2911,7 @@
         <v>5.3815366480765858</v>
       </c>
       <c r="Q21" s="4">
-        <f>Q15*$I$13</f>
+        <f>Q15*$K$13</f>
         <v>5.6772254748939801</v>
       </c>
       <c r="S21" s="8">
@@ -2510,15 +2931,15 @@
         <v>1.0285714285714285</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D22" s="4">
         <f>D16*$H$13</f>
@@ -2537,7 +2958,7 @@
         <v>1.2418930726330581</v>
       </c>
       <c r="Q22" s="4">
-        <f>Q16*$I$13</f>
+        <f>Q16*$K$13</f>
         <v>1.419306368723495</v>
       </c>
       <c r="S22" s="8">
@@ -2557,15 +2978,15 @@
         <v>1.0285714285714285</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D23" s="4">
         <f>D14*(1-$H$13)</f>
@@ -2584,7 +3005,7 @@
         <v>38.952074786078143</v>
       </c>
       <c r="Q23" s="4">
-        <f>Q14*(1-$I$13)</f>
+        <f>Q14*(1-$K$13)</f>
         <v>37.848169832626539</v>
       </c>
       <c r="S23" s="8">
@@ -2604,15 +3025,15 @@
         <v>0.98461538461538467</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D24" s="4">
         <f>D15*(1-$H$13)</f>
@@ -2631,7 +3052,7 @@
         <v>9.994282346427946</v>
       </c>
       <c r="Q24" s="4">
-        <f>Q15*(1-$I$13)</f>
+        <f>Q15*(1-$K$13)</f>
         <v>10.09284528870041</v>
       </c>
       <c r="S24" s="8">
@@ -2651,22 +3072,22 @@
         <v>0.98461538461538456</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D25" s="4">
         <f>D16*(1-$H$13)</f>
         <v>2.5626364990840886</v>
       </c>
       <c r="N25" s="4">
-        <f t="shared" si="5"/>
+        <f>N16*(1-$H$13)</f>
         <v>2.5626364990840886</v>
       </c>
       <c r="O25" s="4">
@@ -2678,7 +3099,7 @@
         <v>2.3063728491756796</v>
       </c>
       <c r="Q25" s="4">
-        <f>Q16*(1-$I$13)</f>
+        <f>Q16*(1-$K$13)</f>
         <v>2.5232113221751025</v>
       </c>
       <c r="S25" s="8">
@@ -2698,81 +3119,81 @@
         <v>0.98461538461538456</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D26" s="4">
-        <f>'Flat glass'!D20</f>
+        <f>'Flat glass'!$D$20</f>
         <v>12.4</v>
       </c>
       <c r="N26" s="4">
-        <f>4.3+2.7+12.5+0.4+0.4+0.1</f>
-        <v>20.399999999999999</v>
+        <f>'Flat glass'!$D$20</f>
+        <v>12.4</v>
       </c>
       <c r="O26" s="4">
-        <f>4.3+2.7+12.5+0.4+0.4+0.1</f>
-        <v>20.399999999999999</v>
+        <f>'Flat glass'!$D$20</f>
+        <v>12.4</v>
       </c>
       <c r="P26" s="4">
-        <f>4.3+2.7+12.5+0.4+0.4+0.1</f>
-        <v>20.399999999999999</v>
+        <f>'Flat glass'!$D$20</f>
+        <v>12.4</v>
       </c>
       <c r="Q26" s="4">
-        <f>4.3+2.7+12.5+0.4+0.4+0.1</f>
-        <v>20.399999999999999</v>
+        <f>'Flat glass'!$D$20</f>
+        <v>12.4</v>
       </c>
       <c r="S26" s="8">
         <f t="shared" si="0"/>
-        <v>1.6451612903225805</v>
+        <v>1</v>
       </c>
       <c r="T26" s="8">
         <f t="shared" si="1"/>
-        <v>1.6451612903225805</v>
+        <v>1</v>
       </c>
       <c r="U26" s="8">
         <f t="shared" si="2"/>
-        <v>1.6451612903225805</v>
+        <v>1</v>
       </c>
       <c r="V26" s="8">
         <f t="shared" si="3"/>
-        <v>1.6451612903225805</v>
-      </c>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D27" s="4">
-        <f>'Flat glass'!D21</f>
+        <f>'Flat glass'!$D$21</f>
         <v>0.77333333333333343</v>
       </c>
       <c r="N27" s="4">
-        <f>(0.15+0.25+0.08+0.1)*100/(15+16+16+28)</f>
+        <f>'Flat glass'!$D$21</f>
         <v>0.77333333333333343</v>
       </c>
       <c r="O27" s="4">
-        <f>(0.15+0.25+0.08+0.1)*100/(15+16+16+28)</f>
+        <f>'Flat glass'!$D$21</f>
         <v>0.77333333333333343</v>
       </c>
       <c r="P27" s="4">
-        <f>(0.15+0.25+0.08+0.1)*100/(15+16+16+28)</f>
+        <f>'Flat glass'!$D$21</f>
         <v>0.77333333333333343</v>
       </c>
       <c r="Q27" s="4">
-        <f>(0.15+0.25+0.08+0.1)*100/(15+16+16+28)</f>
+        <f>'Flat glass'!$D$21</f>
         <v>0.77333333333333343</v>
       </c>
       <c r="S27" s="8">
@@ -2790,356 +3211,6 @@
       <c r="V27" s="8">
         <f t="shared" si="3"/>
         <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="X30" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z30" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB30" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC30" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD30" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="X31" t="str">
-        <f>A9</f>
-        <v>CGM</v>
-      </c>
-      <c r="Y31" t="str">
-        <f>B9</f>
-        <v>loss1</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>91</v>
-      </c>
-      <c r="AA31" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB31" s="9">
-        <f>S9</f>
-        <v>0.92442272756713495</v>
-      </c>
-      <c r="AC31" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD31" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE31" s="9">
-        <f>V9</f>
-        <v>0.98461538461538456</v>
-      </c>
-    </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="X32" t="str">
-        <f t="shared" ref="X32:Y34" si="6">A11</f>
-        <v>FGM</v>
-      </c>
-      <c r="Y32" t="str">
-        <f t="shared" si="6"/>
-        <v>loss2</v>
-      </c>
-      <c r="Z32" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA32" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB32" s="9">
-        <f>S11</f>
-        <v>0.92442272756713506</v>
-      </c>
-      <c r="AC32" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD32" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE32" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="24:31" x14ac:dyDescent="0.25">
-      <c r="X33" t="str">
-        <f t="shared" si="6"/>
-        <v>CGF</v>
-      </c>
-      <c r="Y33" t="str">
-        <f t="shared" si="6"/>
-        <v>CGM</v>
-      </c>
-      <c r="Z33" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA33" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB33" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC33" s="9">
-        <f>T12</f>
-        <v>0.89010989010988961</v>
-      </c>
-      <c r="AD33" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE33" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="24:31" x14ac:dyDescent="0.25">
-      <c r="X34" t="str">
-        <f t="shared" si="6"/>
-        <v>FGF</v>
-      </c>
-      <c r="Y34" t="str">
-        <f t="shared" si="6"/>
-        <v>FGM</v>
-      </c>
-      <c r="Z34" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA34" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB34" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC34" s="9">
-        <f>T13</f>
-        <v>0.92248062015503873</v>
-      </c>
-      <c r="AD34" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE34" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="24:31" x14ac:dyDescent="0.25">
-      <c r="X35" t="str">
-        <f>A16</f>
-        <v>CGF</v>
-      </c>
-      <c r="Y35" t="str">
-        <f>B16</f>
-        <v>CGU</v>
-      </c>
-      <c r="Z35" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA35" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB35" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC35" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD35" s="9">
-        <f>U16</f>
-        <v>0.9</v>
-      </c>
-      <c r="AE35" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="24:31" x14ac:dyDescent="0.25">
-      <c r="X36" t="str">
-        <f t="shared" ref="X36:Y40" si="7">A18</f>
-        <v>FGF</v>
-      </c>
-      <c r="Y36" t="str">
-        <f t="shared" si="7"/>
-        <v>FGU</v>
-      </c>
-      <c r="Z36" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA36" t="s">
-        <v>95</v>
-      </c>
-      <c r="AB36" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC36" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD36" s="9">
-        <f>U18</f>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="AE36" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="24:31" x14ac:dyDescent="0.25">
-      <c r="X37" t="str">
-        <f t="shared" si="7"/>
-        <v>FGF</v>
-      </c>
-      <c r="Y37" t="str">
-        <f t="shared" si="7"/>
-        <v>FGU</v>
-      </c>
-      <c r="Z37" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA37" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB37" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC37" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD37" s="9">
-        <f>U19</f>
-        <v>0.95454545454545447</v>
-      </c>
-      <c r="AE37" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="24:31" x14ac:dyDescent="0.25">
-      <c r="X38" t="str">
-        <f t="shared" si="7"/>
-        <v>CGU</v>
-      </c>
-      <c r="Y38" t="str">
-        <f t="shared" si="7"/>
-        <v>CGM</v>
-      </c>
-      <c r="Z38" t="s">
-        <v>98</v>
-      </c>
-      <c r="AA38" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB38" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC38" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD38" s="9">
-        <f>U20</f>
-        <v>1.0133333333333332</v>
-      </c>
-      <c r="AE38" s="9">
-        <f>V20</f>
-        <v>1.0285714285714287</v>
-      </c>
-    </row>
-    <row r="39" spans="24:31" x14ac:dyDescent="0.25">
-      <c r="X39" t="str">
-        <f t="shared" si="7"/>
-        <v>CGU</v>
-      </c>
-      <c r="Y39" t="str">
-        <f t="shared" si="7"/>
-        <v>CGM</v>
-      </c>
-      <c r="Z39" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA39" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB39" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC39" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD39" s="9">
-        <f>U21</f>
-        <v>0.97500000000000009</v>
-      </c>
-      <c r="AE39" s="9">
-        <f>V21</f>
-        <v>1.0285714285714285</v>
-      </c>
-    </row>
-    <row r="40" spans="24:31" x14ac:dyDescent="0.25">
-      <c r="X40" t="str">
-        <f t="shared" si="7"/>
-        <v>CGU</v>
-      </c>
-      <c r="Y40" t="str">
-        <f t="shared" si="7"/>
-        <v>CGM</v>
-      </c>
-      <c r="Z40" t="s">
-        <v>97</v>
-      </c>
-      <c r="AA40" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB40" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC40" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD40" s="9">
-        <f>U22</f>
-        <v>0.9</v>
-      </c>
-      <c r="AE40" s="9">
-        <f>V22</f>
-        <v>1.0285714285714285</v>
-      </c>
-    </row>
-    <row r="41" spans="24:31" x14ac:dyDescent="0.25">
-      <c r="X41" t="str">
-        <f>A25</f>
-        <v>CGU</v>
-      </c>
-      <c r="Y41" t="str">
-        <f>B25</f>
-        <v>EoL</v>
-      </c>
-      <c r="Z41" t="s">
-        <v>97</v>
-      </c>
-      <c r="AA41" t="s">
-        <v>100</v>
-      </c>
-      <c r="AB41" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC41" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD41" s="9">
-        <f>U25</f>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="AE41" s="9">
-        <f>V25</f>
-        <v>0.98461538461538456</v>
       </c>
     </row>
   </sheetData>
@@ -3161,23 +3232,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C5F011-9BE9-4369-9A3B-10B4B1EB8745}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3195,15 +3266,34 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
+        <f>'Flat glass'!C13</f>
+        <v>2010</v>
+      </c>
+      <c r="C3">
+        <f>'Flat glass'!D13*Flows!H10</f>
+        <v>44.82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2014</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="2">
         <f>Flows!D26</f>
         <v>12.4</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C4" s="2">
         <f>Flows!D17</f>
         <v>58.782946191650787</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2015</v>
+      </c>
+      <c r="C5">
+        <f>'Flat glass'!D4*Flows!H10</f>
+        <v>60.756</v>
       </c>
     </row>
   </sheetData>
@@ -3216,20 +3306,20 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added estimates of emissions and changed edited sankey
</commit_message>
<xml_diff>
--- a/data/glass_paper.xlsx
+++ b/data/glass_paper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Desktop\python\glass-paper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80CD64D-A4B3-443E-8868-43E84FA63DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED85963-2D0A-4A03-9AB4-77C3917927D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-5925" windowWidth="30960" windowHeight="16920" activeTab="5" xr2:uid="{1AC0E601-1297-4C8D-8E5F-6A8C787FDED8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="6" xr2:uid="{1AC0E601-1297-4C8D-8E5F-6A8C787FDED8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mentioned_numbers" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Flows" sheetId="3" r:id="rId4"/>
     <sheet name="Building_flows" sheetId="5" r:id="rId5"/>
     <sheet name="Car_flows" sheetId="6" r:id="rId6"/>
+    <sheet name="Glass_production_by_region" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="147">
   <si>
     <t>Process emissions</t>
   </si>
@@ -395,6 +396,90 @@
   </si>
   <si>
     <t>Global glass emissions in 2014</t>
+  </si>
+  <si>
+    <t>Flat glass production in 2050</t>
+  </si>
+  <si>
+    <t>Container glass production in 2050</t>
+  </si>
+  <si>
+    <t>From stock model</t>
+  </si>
+  <si>
+    <t>Same population data as the transport stock model</t>
+  </si>
+  <si>
+    <t>Population growth</t>
+  </si>
+  <si>
+    <t>Reducing yield losses</t>
+  </si>
+  <si>
+    <t>Diverting manufacturing scrap</t>
+  </si>
+  <si>
+    <t>Reusing components</t>
+  </si>
+  <si>
+    <t>Using less material by design</t>
+  </si>
+  <si>
+    <t>Longer life products</t>
+  </si>
+  <si>
+    <t>Reducing final demand</t>
+  </si>
+  <si>
+    <t>Global glass emissions in 2050</t>
+  </si>
+  <si>
+    <t>Estimates for emission reduction</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Container glass production [Mt]</t>
+  </si>
+  <si>
+    <t>Flat glass production [Mt]</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Russian Federation</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>South America</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Data for 2014 from https://www.sciencedirect.com/science/article/pii/B9780128150603000153</t>
+  </si>
+  <si>
+    <t>South East Asia</t>
+  </si>
+  <si>
+    <t>Rest of the World</t>
+  </si>
+  <si>
+    <t>Rest of the world</t>
   </si>
 </sst>
 </file>
@@ -798,23 +883,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D74802-20F5-460E-AF3A-FC01A078C0A6}">
-  <dimension ref="B2:D11"/>
+  <dimension ref="B2:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>102</v>
       </c>
@@ -825,7 +913,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>103</v>
       </c>
@@ -836,7 +924,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>117</v>
       </c>
@@ -848,7 +936,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>118</v>
       </c>
@@ -860,7 +948,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>110</v>
       </c>
@@ -872,7 +960,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>109</v>
       </c>
@@ -882,6 +970,132 @@
       </c>
       <c r="D11" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="8">
+        <f>9550945000/7243784000</f>
+        <v>1.3185021806282462</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="4">
+        <f>62.866533+10.33176371+Flows!D19*C13</f>
+        <v>83.470102373998657</v>
+      </c>
+      <c r="D15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="4">
+        <f>C13*'Container glass'!D13</f>
+        <v>103.96436345230478</v>
+      </c>
+      <c r="D16" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="4">
+        <f>(C16+C15)*C4</f>
+        <v>106.83764552099295</v>
+      </c>
+      <c r="D18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="8">
+        <f>C18/C7-1</f>
+        <v>0.24789923985554885</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="2">
+        <f>(C16*(1-0.68)+C15)*C4</f>
+        <v>66.541058246879615</v>
+      </c>
+      <c r="D23" s="8">
+        <f>1-C23/C18</f>
+        <v>0.37717592031916591</v>
+      </c>
+      <c r="E23" s="2">
+        <f>D23*$C$18</f>
+        <v>40.296587274113328</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="2">
+        <f>(C16*0.9+C15)*C4</f>
+        <v>100.91167680421158</v>
+      </c>
+      <c r="D24" s="8">
+        <f>1-C24/$C$18</f>
+        <v>5.546704710575967E-2</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" ref="E24:E25" si="0">D24*$C$18</f>
+        <v>5.9259687167813695</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="2">
+        <f>(62.866533+7.14663048+Flows!D19*C13+C16)*C4</f>
+        <v>105.02211957989296</v>
+      </c>
+      <c r="D25" s="8">
+        <f>1-C25/$C$18</f>
+        <v>1.6993316655815383E-2</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8155259410999891</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -889,6 +1103,7 @@
     <hyperlink ref="D9" r:id="rId1" xr:uid="{67A8E8E8-FF10-43BB-AFAA-918C967621FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1705,11 +1920,11 @@
         <v>1</v>
       </c>
       <c r="X4" t="str">
-        <f>A11</f>
+        <f t="shared" ref="X4:Y6" si="4">A11</f>
         <v>FGM</v>
       </c>
       <c r="Y4" t="str">
-        <f>B11</f>
+        <f t="shared" si="4"/>
         <v>loss2</v>
       </c>
       <c r="Z4" t="s">
@@ -1795,11 +2010,11 @@
         <v>0.98461538461538467</v>
       </c>
       <c r="X5" t="str">
-        <f>A12</f>
+        <f t="shared" si="4"/>
         <v>CGF</v>
       </c>
       <c r="Y5" t="str">
-        <f>B12</f>
+        <f t="shared" si="4"/>
         <v>CGM</v>
       </c>
       <c r="Z5" t="s">
@@ -1885,11 +2100,11 @@
         <v>0.98461538461538456</v>
       </c>
       <c r="X6" t="str">
-        <f>A13</f>
+        <f t="shared" si="4"/>
         <v>FGF</v>
       </c>
       <c r="Y6" t="str">
-        <f>B13</f>
+        <f t="shared" si="4"/>
         <v>FGM</v>
       </c>
       <c r="Z6" t="s">
@@ -2065,11 +2280,11 @@
         <v>1</v>
       </c>
       <c r="X8" t="str">
-        <f>A18</f>
+        <f t="shared" ref="X8:Y12" si="5">A18</f>
         <v>FGF</v>
       </c>
       <c r="Y8" t="str">
-        <f>B18</f>
+        <f t="shared" si="5"/>
         <v>FGU</v>
       </c>
       <c r="Z8" t="s">
@@ -2155,11 +2370,11 @@
         <v>0.98461538461538456</v>
       </c>
       <c r="X9" t="str">
-        <f>A19</f>
+        <f t="shared" si="5"/>
         <v>FGF</v>
       </c>
       <c r="Y9" t="str">
-        <f>B19</f>
+        <f t="shared" si="5"/>
         <v>FGU</v>
       </c>
       <c r="Z9" t="s">
@@ -2245,11 +2460,11 @@
         <v>1</v>
       </c>
       <c r="X10" t="str">
-        <f>A20</f>
+        <f t="shared" si="5"/>
         <v>CGU</v>
       </c>
       <c r="Y10" t="str">
-        <f>B20</f>
+        <f t="shared" si="5"/>
         <v>CGM</v>
       </c>
       <c r="Z10" t="s">
@@ -2336,11 +2551,11 @@
         <v>1</v>
       </c>
       <c r="X11" t="str">
-        <f>A21</f>
+        <f t="shared" si="5"/>
         <v>CGU</v>
       </c>
       <c r="Y11" t="str">
-        <f>B21</f>
+        <f t="shared" si="5"/>
         <v>CGM</v>
       </c>
       <c r="Z11" t="s">
@@ -2427,11 +2642,11 @@
         <v>1</v>
       </c>
       <c r="X12" t="str">
-        <f>A22</f>
+        <f t="shared" si="5"/>
         <v>CGU</v>
       </c>
       <c r="Y12" t="str">
-        <f>B22</f>
+        <f t="shared" si="5"/>
         <v>CGM</v>
       </c>
       <c r="Z12" t="s">
@@ -2852,15 +3067,15 @@
         <v>20.698217877217637</v>
       </c>
       <c r="N20" s="4">
-        <f t="shared" ref="N20:P22" si="4">N14*$H$13</f>
+        <f t="shared" ref="N20:P22" si="6">N14*$H$13</f>
         <v>20.698217877217637</v>
       </c>
       <c r="O20" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>20.698217877217637</v>
       </c>
       <c r="P20" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>20.974194115580538</v>
       </c>
       <c r="Q20" s="4">
@@ -2899,15 +3114,15 @@
         <v>5.5195247672580363</v>
       </c>
       <c r="N21" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.5195247672580363</v>
       </c>
       <c r="O21" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.5195247672580363</v>
       </c>
       <c r="P21" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.3815366480765858</v>
       </c>
       <c r="Q21" s="4">
@@ -2946,15 +3161,15 @@
         <v>1.3798811918145091</v>
       </c>
       <c r="N22" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.3798811918145091</v>
       </c>
       <c r="O22" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.3798811918145091</v>
       </c>
       <c r="P22" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.2418930726330581</v>
       </c>
       <c r="Q22" s="4">
@@ -2993,15 +3208,15 @@
         <v>38.439547486261326</v>
       </c>
       <c r="N23" s="4">
-        <f t="shared" ref="N23:P25" si="5">N14*(1-$H$13)</f>
+        <f t="shared" ref="N23:P25" si="7">N14*(1-$H$13)</f>
         <v>38.439547486261326</v>
       </c>
       <c r="O23" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>38.439547486261326</v>
       </c>
       <c r="P23" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>38.952074786078143</v>
       </c>
       <c r="Q23" s="4">
@@ -3040,15 +3255,15 @@
         <v>10.250545996336355</v>
       </c>
       <c r="N24" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>10.250545996336355</v>
       </c>
       <c r="O24" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>10.250545996336355</v>
       </c>
       <c r="P24" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.994282346427946</v>
       </c>
       <c r="Q24" s="4">
@@ -3091,11 +3306,11 @@
         <v>2.5626364990840886</v>
       </c>
       <c r="O25" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.5626364990840886</v>
       </c>
       <c r="P25" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.3063728491756796</v>
       </c>
       <c r="Q25" s="4">
@@ -3305,7 +3520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFBE00B-16BB-4492-A6C9-F4C0D6C72784}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -3351,4 +3566,193 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B548B786-0942-47F7-81F9-DE51894AFDB7}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3">
+        <v>22.1</v>
+      </c>
+      <c r="C3">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D3">
+        <f>B3+C3</f>
+        <v>30.900000000000002</v>
+      </c>
+      <c r="E3" s="8">
+        <f>D3/SUM($D$3:$D$6)</f>
+        <v>0.20571200319552627</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4">
+        <v>13.2</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D14" si="0">B4+C4</f>
+        <v>19.2</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" ref="E4:E6" si="1">D4/SUM($D$3:$D$6)</f>
+        <v>0.12782105052925902</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5">
+        <v>17.32</v>
+      </c>
+      <c r="C5">
+        <v>36.6</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>53.92</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="1"/>
+        <v>0.35896411690300245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6">
+        <f>SUM(B8:B14)</f>
+        <v>24.380000000000003</v>
+      </c>
+      <c r="C6">
+        <f>SUM(C8:C14)</f>
+        <v>21.81</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>46.19</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="1"/>
+        <v>0.30750282937221218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9">
+        <v>3.1539999999999999</v>
+      </c>
+      <c r="C9">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10">
+        <v>2.65</v>
+      </c>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11">
+        <v>2.66</v>
+      </c>
+      <c r="C11">
+        <v>1.5</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12">
+        <v>1.38</v>
+      </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14">
+        <f>77-SUM(B3:B5)-SUM(B8:B12)</f>
+        <v>7.5360000000000014</v>
+      </c>
+      <c r="C14">
+        <v>14.78</v>
+      </c>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added pipenv file, license and readme
</commit_message>
<xml_diff>
--- a/data/glass_paper.xlsx
+++ b/data/glass_paper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Desktop\python\glass-paper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED85963-2D0A-4A03-9AB4-77C3917927D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8477554-1705-49AD-9FEB-4557FCF7BF95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="6" xr2:uid="{1AC0E601-1297-4C8D-8E5F-6A8C787FDED8}"/>
+    <workbookView xWindow="20370" yWindow="-5925" windowWidth="30960" windowHeight="16920" activeTab="1" xr2:uid="{1AC0E601-1297-4C8D-8E5F-6A8C787FDED8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mentioned_numbers" sheetId="1" r:id="rId1"/>
@@ -182,9 +182,6 @@
     <t>Global container glass production [Mt]</t>
   </si>
   <si>
-    <t>Table 11.1: https://www.sciencedirect.com/science/article/pii/B9780128150603000153</t>
-  </si>
-  <si>
     <t>Global container glass production (no USA) [M units]</t>
   </si>
   <si>
@@ -480,6 +477,9 @@
   </si>
   <si>
     <t>Rest of the world</t>
+  </si>
+  <si>
+    <t>Table 11.1: https://www.sciencedirect.com/science/article/pii/B9780123814753100117</t>
   </si>
 </sst>
 </file>
@@ -899,82 +899,82 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C3">
         <v>7.8</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4">
         <v>0.56999999999999995</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6">
         <f>'Container glass'!D3+'Flat glass'!D4</f>
         <v>150.19999999999999</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" s="4">
         <f>C6*C4</f>
         <v>85.61399999999999</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9">
         <f>20.5+11.8</f>
         <v>32.299999999999997</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C11" s="2">
         <f>C7/(C9*1000)*100</f>
         <v>0.26505882352941179</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C13" s="8">
         <f>9550945000/7243784000</f>
@@ -983,44 +983,44 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C15" s="4">
         <f>62.866533+10.33176371+Flows!D19*C13</f>
         <v>83.470102373998657</v>
       </c>
       <c r="D15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C16" s="4">
         <f>C13*'Container glass'!D13</f>
         <v>103.96436345230478</v>
       </c>
       <c r="D16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C18" s="4">
         <f>(C16+C15)*C4</f>
         <v>106.83764552099295</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E18" s="8">
         <f>C18/C7-1</f>
@@ -1029,22 +1029,22 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C23" s="2">
         <f>(C16*(1-0.68)+C15)*C4</f>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C24" s="2">
         <f>(C16*0.9+C15)*C4</f>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C25" s="2">
         <f>(62.866533+7.14663048+Flows!D19*C13+C16)*C4</f>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1111,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED833CB7-39CB-488A-8708-1EAEF1D2FD9A}">
   <dimension ref="B2:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,12 +1159,12 @@
         <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <v>2007</v>
@@ -1179,7 +1179,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6">
         <v>2014</v>
@@ -1209,7 +1209,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8">
         <v>2007</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9">
         <v>2014</v>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10">
         <v>2007</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11">
         <v>2014</v>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="10">
         <v>2014</v>
@@ -1361,7 +1361,7 @@
         <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -1417,7 +1417,7 @@
         <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -1431,7 +1431,7 @@
         <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -1445,7 +1445,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -1475,7 +1475,7 @@
         <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -1539,7 +1539,7 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="10">
         <v>2014</v>
@@ -1554,7 +1554,7 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C19">
         <v>2006</v>
@@ -1564,12 +1564,12 @@
         <v>2.69</v>
       </c>
       <c r="E19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20">
         <v>2014</v>
@@ -1579,12 +1579,12 @@
         <v>12.4</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C21">
         <v>2014</v>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C22">
         <v>2006</v>
@@ -1609,7 +1609,7 @@
         <v>0.23</v>
       </c>
       <c r="E22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
@@ -1645,16 +1645,16 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>56</v>
       </c>
       <c r="G1" t="s">
         <v>22</v>
@@ -1663,42 +1663,42 @@
         <v>0.22409999999999999</v>
       </c>
       <c r="I1" t="s">
+        <v>114</v>
+      </c>
+      <c r="N1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T1" t="s">
+        <v>70</v>
+      </c>
+      <c r="U1" t="s">
+        <v>71</v>
+      </c>
+      <c r="V1" t="s">
+        <v>80</v>
+      </c>
+      <c r="X1" s="13" t="s">
         <v>115</v>
-      </c>
-      <c r="N1" t="s">
-        <v>70</v>
-      </c>
-      <c r="O1" t="s">
-        <v>71</v>
-      </c>
-      <c r="P1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>81</v>
-      </c>
-      <c r="S1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T1" t="s">
-        <v>71</v>
-      </c>
-      <c r="U1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V1" t="s">
-        <v>81</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
         <v>57</v>
-      </c>
-      <c r="B2" t="s">
-        <v>58</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -1714,7 +1714,7 @@
         <v>0.14069999999999999</v>
       </c>
       <c r="I2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N2" s="4">
         <f>(('Flat glass'!$D$18+N11))*$H$1</f>
@@ -1749,36 +1749,36 @@
         <v>1</v>
       </c>
       <c r="X2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y2" t="s">
         <v>53</v>
       </c>
-      <c r="Y2" t="s">
-        <v>54</v>
-      </c>
       <c r="Z2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA2" t="s">
         <v>53</v>
       </c>
-      <c r="AA2" t="s">
-        <v>54</v>
-      </c>
       <c r="AB2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC2" t="s">
         <v>70</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>71</v>
       </c>
-      <c r="AD2" t="s">
-        <v>72</v>
-      </c>
       <c r="AE2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
         <v>57</v>
-      </c>
-      <c r="B3" t="s">
-        <v>58</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -1794,7 +1794,7 @@
         <v>0.63519999999999999</v>
       </c>
       <c r="I3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N3" s="4">
         <f>(('Flat glass'!$D$18+N11))*$H$3</f>
@@ -1837,7 +1837,7 @@
         <v>loss1</v>
       </c>
       <c r="Z3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AA3" t="s">
         <v>0</v>
@@ -1847,10 +1847,10 @@
         <v>0.92442272756713495</v>
       </c>
       <c r="AC3" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AD3" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AE3" s="9">
         <f>V9</f>
@@ -1859,10 +1859,10 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
         <v>57</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -1872,7 +1872,7 @@
         <v>11.788444010275478</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4" t="s">
         <v>28</v>
@@ -1881,7 +1881,7 @@
         <v>0.84530000000000005</v>
       </c>
       <c r="I4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K4" s="5">
         <f>H4+K15</f>
@@ -1928,7 +1928,7 @@
         <v>loss2</v>
       </c>
       <c r="Z4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AA4" t="s">
         <v>0</v>
@@ -1938,21 +1938,21 @@
         <v>0.92442272756713506</v>
       </c>
       <c r="AC4" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AD4" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AE4" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
@@ -1962,7 +1962,7 @@
         <v>13.58776385767761</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
         <v>29</v>
@@ -1971,7 +1971,7 @@
         <v>0.1</v>
       </c>
       <c r="I5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K5" s="5">
         <f>H5-K15</f>
@@ -2018,31 +2018,31 @@
         <v>CGM</v>
       </c>
       <c r="Z5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AA5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB5" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AC5" s="9">
         <f>T12</f>
         <v>0.89010989010988961</v>
       </c>
       <c r="AD5" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AE5" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
@@ -2052,7 +2052,7 @@
         <v>38.513822411409272</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G6" t="s">
         <v>30</v>
@@ -2061,7 +2061,7 @@
         <v>0.15</v>
       </c>
       <c r="I6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K6" s="5">
         <f>H6-K15</f>
@@ -2108,31 +2108,31 @@
         <v>FGM</v>
       </c>
       <c r="Z6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AA6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AB6" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AC6" s="9">
         <f>T13</f>
         <v>0.92248062015503873</v>
       </c>
       <c r="AD6" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AE6" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
         <v>27</v>
@@ -2142,7 +2142,7 @@
         <v>8.5310056884214163</v>
       </c>
       <c r="F7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" t="s">
         <v>31</v>
@@ -2151,7 +2151,7 @@
         <v>0.75</v>
       </c>
       <c r="I7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K7" s="5">
         <f>H7+K15</f>
@@ -2198,41 +2198,41 @@
         <v>CGU</v>
       </c>
       <c r="Z7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AA7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB7" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AC7" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AD7" s="9">
         <f>U16</f>
         <v>0.9</v>
       </c>
       <c r="AE7" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
         <v>59</v>
-      </c>
-      <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
       </c>
       <c r="D8" s="4">
         <f>SUM(D14:D16)/(1-$H$5)</f>
         <v>87.61150424219106</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G8" t="s">
         <v>32</v>
@@ -2241,7 +2241,7 @@
         <v>0.2</v>
       </c>
       <c r="I8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K8" s="7">
         <f>H8-K15/2</f>
@@ -2288,41 +2288,41 @@
         <v>FGU</v>
       </c>
       <c r="Z8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA8" t="s">
         <v>86</v>
       </c>
-      <c r="AA8" t="s">
-        <v>87</v>
-      </c>
       <c r="AB8" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AC8" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AD8" s="9">
         <f>U18</f>
         <v>0.91666666666666663</v>
       </c>
       <c r="AE8" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="4">
         <f>(('Container glass'!$D$13-SUM(D20:D22))/$H$4)*(1-$H$4)</f>
         <v>9.3798619758265307</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G9" t="s">
         <v>33</v>
@@ -2331,7 +2331,7 @@
         <v>0.05</v>
       </c>
       <c r="I9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K9" s="7">
         <f>H9-K15/2</f>
@@ -2378,41 +2378,41 @@
         <v>FGU</v>
       </c>
       <c r="Z9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AA9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AB9" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AC9" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AD9" s="9">
         <f>U19</f>
         <v>0.95454545454545447</v>
       </c>
       <c r="AE9" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="4">
         <f>'Flat glass'!$D$18/(1-$H$6)</f>
         <v>83.320972631680775</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" t="s">
         <v>34</v>
@@ -2421,7 +2421,7 @@
         <v>0.83</v>
       </c>
       <c r="I10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K10" s="5">
         <f>H10+K15</f>
@@ -2468,16 +2468,16 @@
         <v>CGM</v>
       </c>
       <c r="Z10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AA10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB10" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AC10" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AD10" s="9">
         <f>U20</f>
@@ -2490,20 +2490,20 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="4">
         <f>('Flat glass'!$D$18/$H$4)*(1-$H$4)</f>
         <v>12.961423513785473</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G11" t="s">
         <v>35</v>
@@ -2512,7 +2512,7 @@
         <v>0.06</v>
       </c>
       <c r="I11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K11" s="7">
         <f>H11-K15/2</f>
@@ -2559,16 +2559,16 @@
         <v>CGM</v>
       </c>
       <c r="Z11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB11" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AC11" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AD11" s="9">
         <f>U21</f>
@@ -2581,20 +2581,20 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="4">
         <f>(SUM(D14:D16)/(1-$H$5))-SUM(D14:D16)</f>
         <v>8.7611504242191103</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G12" t="s">
         <v>36</v>
@@ -2603,7 +2603,7 @@
         <v>0.11</v>
       </c>
       <c r="I12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K12" s="7">
         <f>H12-K15/2</f>
@@ -2650,16 +2650,16 @@
         <v>CGM</v>
       </c>
       <c r="Z12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AA12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB12" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AC12" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AD12" s="9">
         <f>U22</f>
@@ -2672,20 +2672,20 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="4">
         <f>('Flat glass'!$D$18/(1-$H$6))-'Flat glass'!$D$18</f>
         <v>12.498145894752113</v>
       </c>
       <c r="F13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G13" t="s">
         <v>37</v>
@@ -2694,7 +2694,7 @@
         <v>0.35</v>
       </c>
       <c r="I13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K13" s="6">
         <f>H13+K15</f>
@@ -2741,16 +2741,16 @@
         <v>EoL</v>
       </c>
       <c r="Z13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AA13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AB13" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AC13" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AD13" s="9">
         <f>U25</f>
@@ -2763,10 +2763,10 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -2811,10 +2811,10 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
         <v>39</v>
@@ -2824,7 +2824,7 @@
         <v>15.77007076359439</v>
       </c>
       <c r="J15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K15" s="6">
         <v>0.01</v>
@@ -2864,10 +2864,10 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
         <v>40</v>
@@ -2911,10 +2911,10 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
         <v>41</v>
@@ -2959,10 +2959,10 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
         <v>42</v>
@@ -3007,10 +3007,10 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
         <v>43</v>
@@ -3054,10 +3054,10 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
         <v>38</v>
@@ -3101,10 +3101,10 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
         <v>39</v>
@@ -3148,10 +3148,10 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
         <v>40</v>
@@ -3195,10 +3195,10 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
         <v>38</v>
@@ -3242,10 +3242,10 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
         <v>39</v>
@@ -3289,10 +3289,10 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C25" t="s">
         <v>40</v>
@@ -3336,10 +3336,10 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" t="s">
         <v>66</v>
-      </c>
-      <c r="B26" t="s">
-        <v>67</v>
       </c>
       <c r="C26" t="s">
         <v>41</v>
@@ -3383,10 +3383,10 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" t="s">
         <v>66</v>
-      </c>
-      <c r="B27" t="s">
-        <v>67</v>
       </c>
       <c r="C27" t="s">
         <v>42</v>
@@ -3460,10 +3460,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
         <v>98</v>
-      </c>
-      <c r="C1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3531,10 +3531,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
         <v>98</v>
-      </c>
-      <c r="C1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3572,7 +3572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B548B786-0942-47F7-81F9-DE51894AFDB7}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -3580,23 +3580,23 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" t="s">
         <v>132</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>133</v>
-      </c>
-      <c r="C2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3">
         <v>22.1</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4">
         <v>13.2</v>
@@ -3624,7 +3624,7 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D14" si="0">B4+C4</f>
+        <f t="shared" ref="D4:D6" si="0">B4+C4</f>
         <v>19.2</v>
       </c>
       <c r="E4" s="8">
@@ -3634,7 +3634,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B5">
         <v>17.32</v>
@@ -3653,7 +3653,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B6">
         <f>SUM(B8:B14)</f>
@@ -3674,7 +3674,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -3686,7 +3686,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B9">
         <v>3.1539999999999999</v>
@@ -3697,7 +3697,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B10">
         <v>2.65</v>
@@ -3706,7 +3706,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B11">
         <v>2.66</v>
@@ -3718,7 +3718,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B12">
         <v>1.38</v>
@@ -3727,7 +3727,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C13">
         <v>2.8</v>
@@ -3735,7 +3735,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B14">
         <f>77-SUM(B3:B5)-SUM(B8:B12)</f>

</xml_diff>